<commit_message>
Add 003HAB SRA et SRL
</commit_message>
<xml_diff>
--- a/TNR_JDD/RO/JDD.RO.ACT.xlsx
+++ b/TNR_JDD/RO/JDD.RO.ACT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="228" yWindow="504" windowWidth="19356" windowHeight="8676" activeTab="2"/>
+    <workbookView xWindow="228" yWindow="504" windowWidth="19356" windowHeight="8676" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
@@ -625,12 +625,6 @@
     <t>RO.ACT.001.MAJ.01</t>
   </si>
   <si>
-    <t>upd.RO.ACT.001.MAJ.01.........</t>
-  </si>
-  <si>
-    <t>upd.RO.ACT.001.MAJ.01</t>
-  </si>
-  <si>
     <t>upd.PEPLU</t>
   </si>
   <si>
@@ -638,9 +632,6 @@
   </si>
   <si>
     <t>upd.DIVERS02</t>
-  </si>
-  <si>
-    <t>upd.RO.ACT.001.MAJ.01.A.......</t>
   </si>
   <si>
     <t>upd.GROUPE 3</t>
@@ -1127,6 +1118,15 @@
   </si>
   <si>
     <t>RO.ACT.001.LEC.01.A</t>
+  </si>
+  <si>
+    <t>UPD.RO.ACT.001.MAJ.01.........</t>
+  </si>
+  <si>
+    <t>UPD.RO.ACT.001.MAJ.01</t>
+  </si>
+  <si>
+    <t>UPD.RO.ACT.001.MAJ.01.A.......</t>
   </si>
 </sst>
 </file>
@@ -1834,7 +1834,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="G5" s="34" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
@@ -4886,8 +4886,8 @@
   </sheetPr>
   <dimension ref="A1:BE18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AT9" sqref="AT9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -5072,13 +5072,13 @@
         <v>155</v>
       </c>
       <c r="BC1" s="68" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="BD1" s="68" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="BE1" s="68" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:57">
@@ -5223,10 +5223,10 @@
         <v>163</v>
       </c>
       <c r="BD3" s="67" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="BE3" s="67" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:57" s="74" customFormat="1">
@@ -5346,7 +5346,7 @@
         <v>164</v>
       </c>
       <c r="AV4" s="71" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="AW4" s="71" t="s">
         <v>165</v>
@@ -5497,7 +5497,7 @@
         <v>80</v>
       </c>
       <c r="W6" s="77" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="X6" s="41" t="s">
         <v>179</v>
@@ -5536,7 +5536,7 @@
         <v>181</v>
       </c>
       <c r="AJ6" s="78" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="AK6" s="44" t="s">
         <v>182</v>
@@ -5551,7 +5551,7 @@
         <v>170</v>
       </c>
       <c r="AO6" s="77" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="AP6" s="41" t="s">
         <v>178</v>
@@ -5572,22 +5572,22 @@
         <v>178</v>
       </c>
       <c r="AV6" s="66" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="AW6" s="75" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="AX6" s="41" t="s">
         <v>179</v>
       </c>
       <c r="AY6" s="78" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="AZ6" s="41" t="s">
         <v>181</v>
       </c>
       <c r="BA6" s="78" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="BB6" s="47"/>
       <c r="BC6" s="47"/>
@@ -5662,7 +5662,7 @@
         <v>90</v>
       </c>
       <c r="W7" s="77" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="X7" s="41" t="s">
         <v>179</v>
@@ -5716,7 +5716,7 @@
         <v>170</v>
       </c>
       <c r="AO7" s="77" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="AP7" s="41" t="s">
         <v>178</v>
@@ -5737,10 +5737,10 @@
         <v>178</v>
       </c>
       <c r="AV7" s="66" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="AW7" s="75" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="AX7" s="41" t="s">
         <v>179</v>
@@ -5758,7 +5758,7 @@
         <v>186</v>
       </c>
       <c r="BC7" s="79" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="BD7" s="50" t="s">
         <v>186</v>
@@ -5774,41 +5774,41 @@
       <c r="B8" s="40" t="s">
         <v>198</v>
       </c>
-      <c r="C8" s="41" t="s">
-        <v>199</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>200</v>
-      </c>
-      <c r="F8" s="40" t="s">
-        <v>200</v>
+      <c r="C8" s="78" t="s">
+        <v>338</v>
+      </c>
+      <c r="D8" s="66" t="s">
+        <v>338</v>
+      </c>
+      <c r="E8" s="66" t="s">
+        <v>339</v>
+      </c>
+      <c r="F8" s="66" t="s">
+        <v>339</v>
       </c>
       <c r="G8" s="41" t="s">
         <v>170</v>
       </c>
       <c r="H8" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="I8" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="J8" s="40" t="s">
         <v>201</v>
-      </c>
-      <c r="I8" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="J8" s="40" t="s">
-        <v>203</v>
       </c>
       <c r="K8" s="42">
         <v>12</v>
       </c>
-      <c r="L8" s="41" t="s">
-        <v>204</v>
+      <c r="L8" s="78" t="s">
+        <v>340</v>
       </c>
       <c r="M8" s="40" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="N8" s="40" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="O8" s="40" t="s">
         <v>177</v>
@@ -5835,7 +5835,7 @@
         <v>0</v>
       </c>
       <c r="W8" s="77" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="X8" s="41" t="s">
         <v>179</v>
@@ -5844,7 +5844,7 @@
         <v>170</v>
       </c>
       <c r="Z8" s="40" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AA8" s="40" t="s">
         <v>170</v>
@@ -5877,19 +5877,19 @@
         <v>181</v>
       </c>
       <c r="AK8" s="44" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AL8" s="44" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AM8" s="44" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AN8" s="40" t="s">
         <v>170</v>
       </c>
       <c r="AO8" s="77" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="AP8" s="41" t="s">
         <v>178</v>
@@ -5903,17 +5903,17 @@
       <c r="AS8" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="AT8" s="40" t="s">
-        <v>204</v>
+      <c r="AT8" s="66" t="s">
+        <v>340</v>
       </c>
       <c r="AU8" s="40" t="s">
         <v>178</v>
       </c>
       <c r="AV8" s="66" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="AW8" s="75" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="AX8" s="41" t="s">
         <v>179</v>
@@ -5934,7 +5934,7 @@
     </row>
     <row r="9" spans="1:57">
       <c r="A9" s="65" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B9" s="64" t="s">
         <v>168</v>
@@ -5997,10 +5997,10 @@
     </row>
     <row r="10" spans="1:57">
       <c r="A10" s="39" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -6543,8 +6543,8 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -6581,10 +6581,10 @@
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
       <c r="D2" s="52" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E2" s="52" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -6601,13 +6601,13 @@
         <v>166</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C4" s="52" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E4" s="52" t="s">
         <v>164</v>
@@ -6624,41 +6624,41 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="39" t="s">
-        <v>216</v>
-      </c>
-      <c r="B6" s="40" t="s">
-        <v>170</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>170</v>
+        <v>213</v>
+      </c>
+      <c r="B6" s="66" t="s">
+        <v>332</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>332</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="39" t="s">
-        <v>216</v>
-      </c>
-      <c r="B7" s="40" t="s">
-        <v>170</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>170</v>
+        <v>213</v>
+      </c>
+      <c r="B7" s="66" t="s">
+        <v>332</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>332</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="39" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B8" s="53">
         <v>44562</v>
@@ -6667,15 +6667,15 @@
         <v>45658</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="39" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B9" s="53">
         <v>44562</v>
@@ -6684,41 +6684,41 @@
         <v>46023</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="39" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B10" s="47"/>
       <c r="C10" s="47"/>
       <c r="D10" s="40" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="39" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
       <c r="D11" s="40" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="39" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B12" s="53">
         <v>44927</v>
@@ -6727,10 +6727,10 @@
         <v>46388</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -6810,10 +6810,10 @@
       <c r="B2" s="33"/>
       <c r="C2" s="33"/>
       <c r="D2" s="52" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F2" s="33"/>
     </row>
@@ -6849,7 +6849,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="39" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B6" s="40" t="s">
         <v>170</v>
@@ -6858,10 +6858,10 @@
         <v>170</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F6" s="40" t="s">
         <v>170</v>
@@ -6869,7 +6869,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="39" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B7" s="40" t="s">
         <v>170</v>
@@ -6878,10 +6878,10 @@
         <v>170</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F7" s="40" t="s">
         <v>170</v>
@@ -6889,7 +6889,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="39" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B8" s="53">
         <v>44562</v>
@@ -6898,18 +6898,18 @@
         <v>45658</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="39" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B9" s="53">
         <v>44562</v>
@@ -6918,46 +6918,46 @@
         <v>46023</v>
       </c>
       <c r="D9" s="41" t="s">
+        <v>227</v>
+      </c>
+      <c r="E9" s="40" t="s">
         <v>230</v>
       </c>
-      <c r="E9" s="40" t="s">
-        <v>233</v>
-      </c>
       <c r="F9" s="40" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="39" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B10" s="47"/>
       <c r="C10" s="47"/>
       <c r="D10" s="41" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F10" s="47"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="39" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
       <c r="D11" s="41" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F11" s="47"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="39" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B12" s="53">
         <v>44927</v>
@@ -6966,13 +6966,13 @@
         <v>46388</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F12" s="40" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -7050,11 +7050,11 @@
       <c r="B2" s="33"/>
       <c r="C2" s="33"/>
       <c r="D2" s="34" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E2" s="33"/>
       <c r="F2" s="34" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G2" s="33"/>
       <c r="H2" s="33"/>
@@ -7072,7 +7072,7 @@
       <c r="B3" s="33"/>
       <c r="C3" s="33"/>
       <c r="D3" s="34" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E3" s="33"/>
       <c r="F3" s="33"/>
@@ -7087,10 +7087,10 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="54" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -7143,22 +7143,22 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="39" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C7" s="41">
         <v>0</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G7" s="41" t="s">
         <v>179</v>
@@ -7187,22 +7187,22 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="39" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C8" s="41">
         <v>0</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G8" s="41" t="s">
         <v>179</v>
@@ -7231,22 +7231,22 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="39" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C9" s="41">
         <v>0</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F9" s="40" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G9" s="41" t="s">
         <v>179</v>
@@ -7275,22 +7275,22 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="39" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C10" s="41">
         <v>0</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F10" s="40" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G10" s="41" t="s">
         <v>179</v>
@@ -7319,16 +7319,16 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="39" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
       <c r="D11" s="40" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E11" s="47"/>
       <c r="F11" s="40" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G11" s="47"/>
       <c r="H11" s="47"/>
@@ -7341,16 +7341,16 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="39" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B12" s="47"/>
       <c r="C12" s="47"/>
       <c r="D12" s="40" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E12" s="47"/>
       <c r="F12" s="40" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G12" s="47"/>
       <c r="H12" s="47"/>
@@ -7363,22 +7363,22 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="39" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C13" s="41">
         <v>0</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E13" s="41" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F13" s="40" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G13" s="41" t="s">
         <v>179</v>
@@ -7484,7 +7484,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="57" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C1" s="27" t="s">
         <v>13</v>
@@ -7648,7 +7648,7 @@
         <v>156</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C2" s="33"/>
       <c r="D2" s="34" t="s">
@@ -7895,47 +7895,47 @@
     </row>
     <row r="6" spans="1:54">
       <c r="A6" s="39" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D6" s="60" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F6" s="40" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H6" s="41" t="s">
         <v>170</v>
       </c>
       <c r="I6" s="40" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="J6" s="40" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="K6" s="40" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="L6" s="42">
         <v>28</v>
       </c>
       <c r="M6" s="61"/>
       <c r="N6" s="40" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="O6" s="40" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="P6" s="40" t="s">
         <v>178</v>
@@ -7969,7 +7969,7 @@
         <v>170</v>
       </c>
       <c r="AA6" s="40" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="AB6" s="40" t="s">
         <v>170</v>
@@ -8027,7 +8027,7 @@
         <v>178</v>
       </c>
       <c r="AU6" s="60" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="AV6" s="40" t="s">
         <v>178</v>
@@ -8064,7 +8064,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -8075,13 +8075,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="13.2">
       <c r="A1" s="28" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B1" s="62" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C1" s="62" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.2">
@@ -8089,43 +8089,43 @@
         <v>11</v>
       </c>
       <c r="B2" s="40" t="s">
+        <v>268</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="13.2">
+      <c r="A3" s="66" t="s">
+        <v>331</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>271</v>
       </c>
-      <c r="C2" s="40" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="13.2">
+      <c r="A4" s="66" t="s">
+        <v>331</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="13.2">
-      <c r="A3" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="40" t="s">
+      <c r="C4" s="40" t="s">
         <v>273</v>
       </c>
-      <c r="C3" s="40" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="13.2">
+      <c r="A5" s="66" t="s">
+        <v>331</v>
+      </c>
+      <c r="B5" s="40" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="13.2">
-      <c r="A4" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="40" t="s">
+      <c r="C5" s="40" t="s">
         <v>275</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="13.2">
-      <c r="A5" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>277</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="13.2">
@@ -8133,10 +8133,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="13.2">
@@ -8144,10 +8144,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="13.2">
@@ -8155,10 +8155,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="13.2">
@@ -8166,241 +8166,241 @@
         <v>11</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="13.2">
       <c r="A10" s="40" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="13.2">
       <c r="A11" s="40" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="13.2">
       <c r="A12" s="40" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="13.2">
       <c r="A13" s="40" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="13.2">
       <c r="A14" s="40" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="13.2">
       <c r="A15" s="40" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="13.2">
       <c r="A16" s="40" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="13.2">
       <c r="A17" s="66" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B17" s="66" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C17" s="66" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="13.2">
       <c r="A18" s="66" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B18" s="66" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C18" s="66" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="13.2">
       <c r="A19" s="66" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B19" s="66" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C19" s="66" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="13.2">
       <c r="A20" s="66" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B20" s="66" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C20" s="66" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="13.2">
       <c r="A21" s="66" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B21" s="66" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C21" s="66" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1">
       <c r="A22" s="66" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B22" s="66" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C22" s="66" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1">
       <c r="A23" s="66" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B23" s="66" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C23" s="66" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1">
       <c r="A24" s="66" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B24" s="66" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C24" s="66" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="13.2">
       <c r="A25" s="66" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C25" s="66" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="13.2">
       <c r="A26" s="66" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B26" s="66" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C26" s="66" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" customHeight="1">
       <c r="A27" s="66" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B27" s="66" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C27" s="66" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1">
       <c r="A28" s="66" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B28" s="66" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C28" s="66" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1">
       <c r="A29" s="66" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B29" s="66" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C29" s="66" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1">
       <c r="A30" s="66" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B30" s="66" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C30" s="66" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de MET et de EMP
</commit_message>
<xml_diff>
--- a/TNR_JDD/RO/JDD.RO.ACT.xlsx
+++ b/TNR_JDD/RO/JDD.RO.ACT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="228" yWindow="504" windowWidth="19356" windowHeight="8676" activeTab="4"/>
+    <workbookView xWindow="228" yWindow="504" windowWidth="19356" windowHeight="8676" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="377">
   <si>
     <t>Date</t>
   </si>
@@ -805,12 +805,6 @@
     <t>N5</t>
   </si>
   <si>
-    <t>RT.EMP*001*ST_CODLON</t>
-  </si>
-  <si>
-    <t>ID_NUMEMP*EMP*ST_CODLON</t>
-  </si>
-  <si>
     <t>SEQUENCE</t>
   </si>
   <si>
@@ -1255,6 +1249,72 @@
   </si>
   <si>
     <t>SelectionMetier_input_ST_NIV</t>
+  </si>
+  <si>
+    <t>zon3</t>
+  </si>
+  <si>
+    <t>RT.EMP*001*ST_CODCOU</t>
+  </si>
+  <si>
+    <t>ID_NUMEMP*EMP*ST_CODCOU</t>
+  </si>
+  <si>
+    <t>004EMP</t>
+  </si>
+  <si>
+    <t>a_AjouterEmplacement</t>
+  </si>
+  <si>
+    <t>span_Supprime_Emplacement</t>
+  </si>
+  <si>
+    <t>SelectionEmplacement_input_Filtre</t>
+  </si>
+  <si>
+    <t>SelectionEmplacement_td</t>
+  </si>
+  <si>
+    <t>SelectionEmplacement_button_Ajouter</t>
+  </si>
+  <si>
+    <t>//div[@id='grid_AddEMP']//input[@name='SEARCH_ST_CODCOU']</t>
+  </si>
+  <si>
+    <t>//div[@id='bAddGridinterZonLig']/a[@id='add']</t>
+  </si>
+  <si>
+    <t>//div[@id='empFooter']//button[@value='Ajouter']</t>
+  </si>
+  <si>
+    <t>SelectionEmplacement_button_Fermer</t>
+  </si>
+  <si>
+    <t>//div[@id='empFooter']//button[@value='Fermer']</t>
+  </si>
+  <si>
+    <t>//div[@id='v-dbtdhtmlxinterZonLig']/table/tbody//td[5][text()='${ID_NUMREF}']</t>
+  </si>
+  <si>
+    <t>//div[@id='v-dbtdhtmlxinterZonLig']/table/tbody//td[5][text()='${ID_NUMREF}']/preceding-sibling::td[1]/img</t>
+  </si>
+  <si>
+    <t>//div[@id='v-dbtdhtmlxinterZonLig']/table/tbody//td[5][text()='${ID_NUMREF}']/preceding-sibling::td[2]/span</t>
+  </si>
+  <si>
+    <t>//div[@id='v-dbtdhtmlxAddEMP']/table/tbody//td[4][text()='${ID_NUMREF}']</t>
+  </si>
+  <si>
+    <t>//div[@id='v-dbtdhtmlxinterZonLig']/table/tbody//td[5][text()='${ID_NUMREF}']/following-sibling::td[4]</t>
+  </si>
+  <si>
+    <t>//div[@id='v-dbtdhtmlxinterZonLig']/table/tbody//td[5][text()='${ID_NUMREF}']/following-sibling::td[5]</t>
+  </si>
+  <si>
+    <t>//div[@id='v-dbtdhtmlxinterZonLig']/table/tbody//td[5][text()='${ID_NUMREF}']/following-sibling::td[4]/textarea</t>
+  </si>
+  <si>
+    <t>//div[@id='v-dbtdhtmlxinterZonLig']/table/tbody//td[5][text()='${ID_NUMREF}']/following-sibling::td[5]/textarea</t>
   </si>
 </sst>
 </file>
@@ -1369,7 +1429,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1514,6 +1574,18 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1549,7 +1621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1726,12 +1798,20 @@
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0066"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -2002,7 +2082,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="G5" s="34" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1">
@@ -5054,8 +5134,8 @@
   </sheetPr>
   <dimension ref="A1:BE18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="AV13" sqref="AV13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -5240,13 +5320,13 @@
         <v>155</v>
       </c>
       <c r="BC1" s="68" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="BD1" s="68" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="BE1" s="68" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:57">
@@ -5378,7 +5458,9 @@
       <c r="AS3" s="33"/>
       <c r="AT3" s="33"/>
       <c r="AU3" s="33"/>
-      <c r="AV3" s="34"/>
+      <c r="AV3" s="34" t="s">
+        <v>327</v>
+      </c>
       <c r="AW3" s="33"/>
       <c r="AX3" s="33"/>
       <c r="AY3" s="33"/>
@@ -5391,10 +5473,10 @@
         <v>163</v>
       </c>
       <c r="BD3" s="67" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="BE3" s="67" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:57" s="74" customFormat="1">
@@ -5514,7 +5596,7 @@
         <v>164</v>
       </c>
       <c r="AV4" s="71" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AW4" s="71" t="s">
         <v>165</v>
@@ -5665,7 +5747,7 @@
         <v>80</v>
       </c>
       <c r="W6" s="77" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="X6" s="41" t="s">
         <v>179</v>
@@ -5704,7 +5786,7 @@
         <v>181</v>
       </c>
       <c r="AJ6" s="78" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AK6" s="44" t="s">
         <v>182</v>
@@ -5719,7 +5801,7 @@
         <v>170</v>
       </c>
       <c r="AO6" s="77" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AP6" s="41" t="s">
         <v>178</v>
@@ -5739,23 +5821,23 @@
       <c r="AU6" s="40" t="s">
         <v>178</v>
       </c>
-      <c r="AV6" s="66">
-        <v>0</v>
+      <c r="AV6" s="89" t="s">
+        <v>355</v>
       </c>
       <c r="AW6" s="75" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="AX6" s="41" t="s">
         <v>179</v>
       </c>
       <c r="AY6" s="78" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AZ6" s="41" t="s">
         <v>181</v>
       </c>
       <c r="BA6" s="78" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="BB6" s="47"/>
       <c r="BC6" s="47"/>
@@ -5830,7 +5912,7 @@
         <v>90</v>
       </c>
       <c r="W7" s="77" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="X7" s="41" t="s">
         <v>179</v>
@@ -5884,7 +5966,7 @@
         <v>170</v>
       </c>
       <c r="AO7" s="77" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AP7" s="41" t="s">
         <v>178</v>
@@ -5908,7 +5990,7 @@
         <v>0</v>
       </c>
       <c r="AW7" s="75" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="AX7" s="41" t="s">
         <v>179</v>
@@ -5926,7 +6008,7 @@
         <v>186</v>
       </c>
       <c r="BC7" s="79" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="BD7" s="50" t="s">
         <v>186</v>
@@ -5943,16 +6025,16 @@
         <v>198</v>
       </c>
       <c r="C8" s="78" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D8" s="66" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E8" s="66" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F8" s="66" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G8" s="41" t="s">
         <v>170</v>
@@ -5970,7 +6052,7 @@
         <v>12</v>
       </c>
       <c r="L8" s="78" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M8" s="40" t="s">
         <v>202</v>
@@ -6003,7 +6085,7 @@
         <v>0</v>
       </c>
       <c r="W8" s="77" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="X8" s="41" t="s">
         <v>179</v>
@@ -6057,7 +6139,7 @@
         <v>170</v>
       </c>
       <c r="AO8" s="77" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AP8" s="41" t="s">
         <v>178</v>
@@ -6072,7 +6154,7 @@
         <v>178</v>
       </c>
       <c r="AT8" s="66" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="AU8" s="40" t="s">
         <v>178</v>
@@ -6081,7 +6163,7 @@
         <v>0</v>
       </c>
       <c r="AW8" s="75" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="AX8" s="41" t="s">
         <v>179</v>
@@ -6799,10 +6881,10 @@
         <v>214</v>
       </c>
       <c r="D6" s="66" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E6" s="66" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -6816,10 +6898,10 @@
         <v>215</v>
       </c>
       <c r="D7" s="66" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E7" s="66" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -6939,8 +7021,8 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -7000,16 +7082,16 @@
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="85" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D4" s="85" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E4" s="85" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F4" s="85" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -7033,13 +7115,13 @@
         <v>223</v>
       </c>
       <c r="D6" s="66" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E6" s="66" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F6" s="66" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -7053,13 +7135,13 @@
         <v>224</v>
       </c>
       <c r="D7" s="66" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E7" s="66" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F7" s="66" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -7162,8 +7244,8 @@
   </sheetPr>
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -7171,7 +7253,7 @@
     <col min="1" max="1" width="22.21875" customWidth="1"/>
     <col min="2" max="2" width="16.88671875" customWidth="1"/>
     <col min="4" max="4" width="26.109375" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -7184,7 +7266,7 @@
       <c r="C1" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="76" t="s">
         <v>142</v>
       </c>
       <c r="E1" s="28" t="s">
@@ -7225,7 +7307,7 @@
       <c r="B2" s="33"/>
       <c r="C2" s="33"/>
       <c r="D2" s="34" t="s">
-        <v>233</v>
+        <v>356</v>
       </c>
       <c r="E2" s="33"/>
       <c r="F2" s="34" t="s">
@@ -7247,7 +7329,7 @@
       <c r="B3" s="33"/>
       <c r="C3" s="33"/>
       <c r="D3" s="34" t="s">
-        <v>234</v>
+        <v>357</v>
       </c>
       <c r="E3" s="33"/>
       <c r="F3" s="33"/>
@@ -7262,10 +7344,10 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="54" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -7286,13 +7368,21 @@
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
+      <c r="D5" s="34" t="s">
+        <v>369</v>
+      </c>
       <c r="E5" s="33"/>
       <c r="F5" s="33"/>
       <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
+      <c r="H5" s="34" t="s">
+        <v>375</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>376</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>370</v>
+      </c>
       <c r="K5" s="33"/>
       <c r="L5" s="33"/>
       <c r="M5" s="33"/>
@@ -7318,31 +7408,31 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="39" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C7" s="41">
         <v>0</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G7" s="41" t="s">
         <v>179</v>
       </c>
-      <c r="H7" s="40" t="s">
-        <v>170</v>
-      </c>
-      <c r="I7" s="40" t="s">
-        <v>170</v>
+      <c r="H7" s="66" t="s">
+        <v>325</v>
+      </c>
+      <c r="I7" s="66" t="s">
+        <v>325</v>
       </c>
       <c r="J7" s="41" t="s">
         <v>177</v>
@@ -7362,31 +7452,31 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="39" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C8" s="41">
         <v>0</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G8" s="41" t="s">
         <v>179</v>
       </c>
-      <c r="H8" s="40" t="s">
-        <v>170</v>
-      </c>
-      <c r="I8" s="40" t="s">
-        <v>170</v>
+      <c r="H8" s="66" t="s">
+        <v>325</v>
+      </c>
+      <c r="I8" s="66" t="s">
+        <v>325</v>
       </c>
       <c r="J8" s="41" t="s">
         <v>178</v>
@@ -7406,22 +7496,22 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="39" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C9" s="41">
         <v>0</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E9" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="F9" s="40" t="s">
         <v>240</v>
-      </c>
-      <c r="F9" s="40" t="s">
-        <v>242</v>
       </c>
       <c r="G9" s="41" t="s">
         <v>179</v>
@@ -7450,22 +7540,22 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="39" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C10" s="41">
         <v>0</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E10" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="F10" s="40" t="s">
         <v>240</v>
-      </c>
-      <c r="F10" s="40" t="s">
-        <v>242</v>
       </c>
       <c r="G10" s="41" t="s">
         <v>179</v>
@@ -7494,16 +7584,16 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="39" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
       <c r="D11" s="40" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E11" s="47"/>
       <c r="F11" s="40" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G11" s="47"/>
       <c r="H11" s="47"/>
@@ -7516,16 +7606,16 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="39" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B12" s="47"/>
       <c r="C12" s="47"/>
       <c r="D12" s="40" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E12" s="47"/>
       <c r="F12" s="40" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G12" s="47"/>
       <c r="H12" s="47"/>
@@ -7538,22 +7628,22 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="39" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C13" s="41">
         <v>0</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E13" s="41" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F13" s="40" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G13" s="41" t="s">
         <v>179</v>
@@ -7659,7 +7749,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="57" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C1" s="27" t="s">
         <v>13</v>
@@ -8070,47 +8160,47 @@
     </row>
     <row r="6" spans="1:54">
       <c r="A6" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>250</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="D6" s="60" t="s">
         <v>251</v>
       </c>
-      <c r="B6" s="40" t="s">
-        <v>252</v>
-      </c>
-      <c r="C6" s="40" t="s">
+      <c r="E6" s="60" t="s">
         <v>251</v>
       </c>
-      <c r="D6" s="60" t="s">
-        <v>253</v>
-      </c>
-      <c r="E6" s="60" t="s">
-        <v>253</v>
-      </c>
       <c r="F6" s="40" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H6" s="41" t="s">
         <v>170</v>
       </c>
       <c r="I6" s="40" t="s">
+        <v>252</v>
+      </c>
+      <c r="J6" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="K6" s="40" t="s">
         <v>254</v>
-      </c>
-      <c r="J6" s="40" t="s">
-        <v>255</v>
-      </c>
-      <c r="K6" s="40" t="s">
-        <v>256</v>
       </c>
       <c r="L6" s="42">
         <v>28</v>
       </c>
       <c r="M6" s="61"/>
       <c r="N6" s="40" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="O6" s="40" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="P6" s="40" t="s">
         <v>178</v>
@@ -8144,7 +8234,7 @@
         <v>170</v>
       </c>
       <c r="AA6" s="40" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="AB6" s="40" t="s">
         <v>170</v>
@@ -8202,7 +8292,7 @@
         <v>178</v>
       </c>
       <c r="AU6" s="60" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="AV6" s="40" t="s">
         <v>178</v>
@@ -8236,27 +8326,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
-    <col min="3" max="3" width="77.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="13.2">
       <c r="A1" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" s="62" t="s">
+        <v>260</v>
+      </c>
+      <c r="C1" s="62" t="s">
         <v>261</v>
-      </c>
-      <c r="B1" s="62" t="s">
-        <v>262</v>
-      </c>
-      <c r="C1" s="62" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.2">
@@ -8264,43 +8354,43 @@
         <v>11</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="13.2">
       <c r="A3" s="66" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13.2">
       <c r="A4" s="66" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="13.2">
       <c r="A5" s="66" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="13.2">
@@ -8308,10 +8398,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="13.2">
@@ -8319,10 +8409,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="13.2">
@@ -8330,10 +8420,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="13.2">
@@ -8341,329 +8431,424 @@
         <v>11</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="13.2">
       <c r="A10" s="86" t="s">
+        <v>278</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>279</v>
+      </c>
+      <c r="C10" s="66" t="s">
         <v>280</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>281</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="13.2">
       <c r="A11" s="86" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="13.2">
       <c r="A12" s="86" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="13.2">
       <c r="A13" s="86" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="13.2">
       <c r="A14" s="86" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="13.2">
       <c r="A15" s="86" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="13.2">
       <c r="A16" s="86" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C16" s="82" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="13.2">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="13.2">
       <c r="A17" s="87" t="s">
+        <v>334</v>
+      </c>
+      <c r="B17" s="66" t="s">
+        <v>335</v>
+      </c>
+      <c r="C17" s="66" t="s">
         <v>336</v>
       </c>
-      <c r="B17" s="66" t="s">
+    </row>
+    <row r="18" spans="1:5" ht="13.2">
+      <c r="A18" s="87" t="s">
+        <v>334</v>
+      </c>
+      <c r="B18" s="66" t="s">
+        <v>343</v>
+      </c>
+      <c r="C18" s="66" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="13.2">
+      <c r="A19" s="87" t="s">
+        <v>334</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>284</v>
+      </c>
+      <c r="C19" s="66" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="13.2">
+      <c r="A20" s="87" t="s">
+        <v>334</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>286</v>
+      </c>
+      <c r="C20" s="66" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="13.2">
+      <c r="A21" s="87" t="s">
+        <v>334</v>
+      </c>
+      <c r="B21" s="82" t="s">
         <v>337</v>
       </c>
-      <c r="C17" s="66" t="s">
+      <c r="C21" s="82" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="13.2">
+      <c r="A22" s="87" t="s">
+        <v>334</v>
+      </c>
+      <c r="B22" s="82" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="13.2">
-      <c r="A18" s="87" t="s">
-        <v>336</v>
-      </c>
-      <c r="B18" s="66" t="s">
-        <v>345</v>
-      </c>
-      <c r="C18" s="66" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="13.2">
-      <c r="A19" s="87" t="s">
-        <v>336</v>
-      </c>
-      <c r="B19" s="48" t="s">
+      <c r="C22" s="82" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="13.2">
+      <c r="A23" s="87" t="s">
+        <v>334</v>
+      </c>
+      <c r="B23" s="82" t="s">
+        <v>354</v>
+      </c>
+      <c r="C23" s="82" t="s">
+        <v>353</v>
+      </c>
+      <c r="E23" s="91"/>
+    </row>
+    <row r="24" spans="1:5" ht="13.2">
+      <c r="A24" s="87" t="s">
+        <v>334</v>
+      </c>
+      <c r="B24" s="82" t="s">
+        <v>339</v>
+      </c>
+      <c r="C24" s="82" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="13.2">
+      <c r="A25" s="90" t="s">
+        <v>358</v>
+      </c>
+      <c r="B25" s="66" t="s">
+        <v>359</v>
+      </c>
+      <c r="C25" s="92" t="s">
+        <v>365</v>
+      </c>
+      <c r="E25" s="91" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="13.2">
+      <c r="A26" s="90" t="s">
+        <v>358</v>
+      </c>
+      <c r="B26" s="66" t="s">
+        <v>360</v>
+      </c>
+      <c r="C26" s="66" t="s">
+        <v>371</v>
+      </c>
+      <c r="D26" s="66"/>
+      <c r="E26" s="91"/>
+    </row>
+    <row r="27" spans="1:5" ht="13.2">
+      <c r="A27" s="90" t="s">
+        <v>358</v>
+      </c>
+      <c r="B27" s="48" t="s">
+        <v>284</v>
+      </c>
+      <c r="C27" s="66" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="13.2">
+      <c r="A28" s="90" t="s">
+        <v>358</v>
+      </c>
+      <c r="B28" s="48" t="s">
         <v>286</v>
       </c>
-      <c r="C19" s="66" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="13.2">
-      <c r="A20" s="87" t="s">
-        <v>336</v>
-      </c>
-      <c r="B20" s="48" t="s">
-        <v>288</v>
-      </c>
-      <c r="C20" s="66" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="13.2">
-      <c r="A21" s="87" t="s">
-        <v>336</v>
-      </c>
-      <c r="B21" s="82" t="s">
-        <v>339</v>
-      </c>
-      <c r="C21" s="82" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="13.2">
-      <c r="A22" s="87" t="s">
-        <v>336</v>
-      </c>
-      <c r="B22" s="82" t="s">
-        <v>340</v>
-      </c>
-      <c r="C22" s="82" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="13.2">
-      <c r="A23" s="87" t="s">
-        <v>336</v>
-      </c>
-      <c r="B23" s="82" t="s">
-        <v>356</v>
-      </c>
-      <c r="C23" s="66" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="13.2">
-      <c r="A24" s="87" t="s">
-        <v>336</v>
-      </c>
-      <c r="B24" s="82" t="s">
-        <v>341</v>
-      </c>
-      <c r="C24" s="82" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="13.2">
-      <c r="A25" s="66" t="s">
-        <v>326</v>
-      </c>
-      <c r="B25" s="66" t="s">
-        <v>304</v>
-      </c>
-      <c r="C25" s="66" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="13.2">
-      <c r="A26" s="66" t="s">
-        <v>326</v>
-      </c>
-      <c r="B26" s="66" t="s">
-        <v>305</v>
-      </c>
-      <c r="C26" s="66" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="13.2">
-      <c r="A27" s="66" t="s">
-        <v>326</v>
-      </c>
-      <c r="B27" s="66" t="s">
-        <v>296</v>
-      </c>
-      <c r="C27" s="66" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="13.2">
-      <c r="A28" s="66" t="s">
-        <v>326</v>
-      </c>
-      <c r="B28" s="66" t="s">
-        <v>319</v>
-      </c>
       <c r="C28" s="66" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="13.2">
-      <c r="A29" s="66" t="s">
-        <v>326</v>
-      </c>
-      <c r="B29" s="66" t="s">
-        <v>300</v>
-      </c>
-      <c r="C29" s="66" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1">
-      <c r="A30" s="66" t="s">
-        <v>326</v>
-      </c>
-      <c r="B30" s="66" t="s">
-        <v>320</v>
-      </c>
-      <c r="C30" s="66" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15" customHeight="1">
-      <c r="A31" s="66" t="s">
-        <v>326</v>
-      </c>
-      <c r="B31" s="66" t="s">
-        <v>301</v>
-      </c>
-      <c r="C31" s="66" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15" customHeight="1">
-      <c r="A32" s="66" t="s">
-        <v>326</v>
-      </c>
-      <c r="B32" s="66" t="s">
-        <v>325</v>
-      </c>
-      <c r="C32" s="66" t="s">
-        <v>312</v>
+        <v>374</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="13.2">
+      <c r="A29" s="90" t="s">
+        <v>358</v>
+      </c>
+      <c r="B29" s="82" t="s">
+        <v>361</v>
+      </c>
+      <c r="C29" s="82" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="13.2">
+      <c r="A30" s="90" t="s">
+        <v>358</v>
+      </c>
+      <c r="B30" s="82" t="s">
+        <v>362</v>
+      </c>
+      <c r="C30" s="82" t="s">
+        <v>372</v>
+      </c>
+      <c r="E30" s="48"/>
+    </row>
+    <row r="31" spans="1:5" ht="13.2">
+      <c r="A31" s="90" t="s">
+        <v>358</v>
+      </c>
+      <c r="B31" s="82" t="s">
+        <v>363</v>
+      </c>
+      <c r="C31" s="82" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="13.2">
+      <c r="A32" s="90" t="s">
+        <v>358</v>
+      </c>
+      <c r="B32" s="82" t="s">
+        <v>367</v>
+      </c>
+      <c r="C32" s="82" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="13.2">
       <c r="A33" s="66" t="s">
-        <v>326</v>
-      </c>
-      <c r="B33" s="40" t="s">
-        <v>283</v>
+        <v>324</v>
+      </c>
+      <c r="B33" s="66" t="s">
+        <v>302</v>
       </c>
       <c r="C33" s="66" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="13.2">
       <c r="A34" s="66" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B34" s="66" t="s">
+        <v>303</v>
+      </c>
+      <c r="C34" s="66" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="13.2">
+      <c r="A35" s="66" t="s">
         <v>324</v>
       </c>
-      <c r="C34" s="66" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1">
-      <c r="A35" s="66" t="s">
-        <v>326</v>
-      </c>
       <c r="B35" s="66" t="s">
-        <v>321</v>
+        <v>294</v>
       </c>
       <c r="C35" s="66" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="13.2">
       <c r="A36" s="66" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B36" s="66" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C36" s="66" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15" customHeight="1">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="13.2">
       <c r="A37" s="66" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B37" s="66" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C37" s="66" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15" customHeight="1">
       <c r="A38" s="66" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B38" s="66" t="s">
+        <v>318</v>
+      </c>
+      <c r="C38" s="66" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15" customHeight="1">
+      <c r="A39" s="66" t="s">
+        <v>324</v>
+      </c>
+      <c r="B39" s="66" t="s">
+        <v>299</v>
+      </c>
+      <c r="C39" s="66" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15" customHeight="1">
+      <c r="A40" s="66" t="s">
+        <v>324</v>
+      </c>
+      <c r="B40" s="66" t="s">
+        <v>323</v>
+      </c>
+      <c r="C40" s="66" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="13.2">
+      <c r="A41" s="66" t="s">
+        <v>324</v>
+      </c>
+      <c r="B41" s="40" t="s">
+        <v>281</v>
+      </c>
+      <c r="C41" s="66" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="13.2">
+      <c r="A42" s="66" t="s">
+        <v>324</v>
+      </c>
+      <c r="B42" s="66" t="s">
         <v>322</v>
       </c>
-      <c r="C38" s="66" t="s">
-        <v>318</v>
+      <c r="C42" s="66" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15" customHeight="1">
+      <c r="A43" s="66" t="s">
+        <v>324</v>
+      </c>
+      <c r="B43" s="66" t="s">
+        <v>319</v>
+      </c>
+      <c r="C43" s="66" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" customHeight="1">
+      <c r="A44" s="66" t="s">
+        <v>324</v>
+      </c>
+      <c r="B44" s="66" t="s">
+        <v>321</v>
+      </c>
+      <c r="C44" s="66" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" customHeight="1">
+      <c r="A45" s="66" t="s">
+        <v>324</v>
+      </c>
+      <c r="B45" s="66" t="s">
+        <v>300</v>
+      </c>
+      <c r="C45" s="66" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15" customHeight="1">
+      <c r="A46" s="66" t="s">
+        <v>324</v>
+      </c>
+      <c r="B46" s="66" t="s">
+        <v>320</v>
+      </c>
+      <c r="C46" s="66" t="s">
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout log.addSTEPLOOP + corrections
</commit_message>
<xml_diff>
--- a/TNR_JDD/RO/JDD.RO.ACT.xlsx
+++ b/TNR_JDD/RO/JDD.RO.ACT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="612" yWindow="588" windowWidth="21852" windowHeight="8940" activeTab="2"/>
+    <workbookView xWindow="612" yWindow="588" windowWidth="21852" windowHeight="8940" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="394">
   <si>
     <t>Date</t>
   </si>
@@ -865,9 +865,6 @@
     <t>RO.ACT.005.FON.01.............</t>
   </si>
   <si>
-    <t>$VIDE</t>
-  </si>
-  <si>
     <t>PABOCOU</t>
   </si>
   <si>
@@ -1093,85 +1090,124 @@
     <t>a_Acteur</t>
   </si>
   <si>
-    <t>//li[@class ='nav-item']//a[@ml-text3='ID_CODINT']</t>
-  </si>
-  <si>
     <t>a_ActeurSelected</t>
   </si>
   <si>
-    <t>//li[@class ='nav-item']//a[@ml-text3='ID_CODINT' and starts-with(@class,'nav-link active')]</t>
-  </si>
-  <si>
     <t>a_Affectation</t>
   </si>
   <si>
-    <t>//li[@class ='nav-item']//a[@ml-text3='affectation']</t>
-  </si>
-  <si>
     <t>a_AffectationSelected</t>
   </si>
   <si>
-    <t>//li[@class ='nav-item']//a[@ml-text3='affectation' and starts-with(@class,'nav-link active')]</t>
-  </si>
-  <si>
     <t>a_Role</t>
   </si>
   <si>
-    <t>//li[@class ='nav-item']//a[@ml-text3='role']</t>
-  </si>
-  <si>
     <t>a_RoleSelected</t>
   </si>
   <si>
-    <t>//li[@class ='nav-item']//a[@ml-text3='role' and starts-with(@class,'nav-link active')]</t>
-  </si>
-  <si>
     <t>a_Preventif</t>
   </si>
   <si>
-    <t>//li[@class ='nav-item']//a[@ml-text3='preventif']</t>
-  </si>
-  <si>
     <t>a_PreventifSelected</t>
   </si>
   <si>
-    <t>//li[@class ='nav-item']//a[@ml-text3='preventif' and starts-with(@class,'nav-link active')]</t>
-  </si>
-  <si>
     <t>a_Habilitation</t>
   </si>
   <si>
-    <t>//li[@class ='nav-item']//a[@ml-text3='ID_CODHAB']</t>
-  </si>
-  <si>
     <t>a_HabilitationSelected</t>
   </si>
   <si>
-    <t>//li[@class ='nav-item']//a[@ml-text3='ID_CODHAB' and starts-with(@class,'nav-link active')]</t>
-  </si>
-  <si>
     <t>a_Metier</t>
   </si>
   <si>
-    <t>//li[@class ='nav-item']//a[@ml-text3='ID_CODMET']</t>
-  </si>
-  <si>
     <t>a_MetierSelected</t>
   </si>
   <si>
-    <t>//li[@class ='nav-item']//a[@ml-text3='ID_CODMET' and starts-with(@class,'nav-link active')]</t>
-  </si>
-  <si>
     <t>a_Zone</t>
   </si>
   <si>
-    <t>//li[@class ='nav-item']//a[@ml-text3='ID_NUMZON']</t>
-  </si>
-  <si>
     <t>a_ZoneSelected</t>
   </si>
   <si>
-    <t>//li[@class ='nav-item']//a[@ml-text3='ID_NUMZON' and starts-with(@class,'nav-link active')]</t>
+    <t>01010128</t>
+  </si>
+  <si>
+    <t>06060628</t>
+  </si>
+  <si>
+    <t>09090928</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>a_Copy</t>
+  </si>
+  <si>
+    <t>//li[@id='FormE21__copy']/a</t>
+  </si>
+  <si>
+    <t>//li[@class ='nav-item']/a[@ml-text3='ID_CODINT']</t>
+  </si>
+  <si>
+    <t>//li[@class ='nav-item']/a[@ml-text3='ID_CODINT' and starts-with(@class,'nav-link active')]</t>
+  </si>
+  <si>
+    <t>//li[@class ='nav-item']/a[@ml-text3='affectation']</t>
+  </si>
+  <si>
+    <t>//li[@class ='nav-item']/a[@ml-text3='affectation' and starts-with(@class,'nav-link active')]</t>
+  </si>
+  <si>
+    <t>//li[@class ='nav-item']/a[@ml-text3='role']</t>
+  </si>
+  <si>
+    <t>//li[@class ='nav-item']/a[@ml-text3='role' and starts-with(@class,'nav-link active')]</t>
+  </si>
+  <si>
+    <t>//li[@class ='nav-item']/a[@ml-text3='preventif']</t>
+  </si>
+  <si>
+    <t>//li[@class ='nav-item']/a[@ml-text3='preventif' and starts-with(@class,'nav-link active')]</t>
+  </si>
+  <si>
+    <t>//li[@class ='nav-item']/a[@ml-text3='ID_CODHAB']</t>
+  </si>
+  <si>
+    <t>//li[@class ='nav-item']/a[@ml-text3='ID_CODHAB' and starts-with(@class,'nav-link active')]</t>
+  </si>
+  <si>
+    <t>//li[@class ='nav-item']/a[@ml-text3='ID_CODMET']</t>
+  </si>
+  <si>
+    <t>//li[@class ='nav-item']/a[@ml-text3='ID_CODMET' and starts-with(@class,'nav-link active')]</t>
+  </si>
+  <si>
+    <t>//li[@class ='nav-item']/a[@ml-text3='ID_NUMZON']</t>
+  </si>
+  <si>
+    <t>//li[@class ='nav-item']/a[@ml-text3='ID_NUMZON' and starts-with(@class,'nav-link active')]</t>
+  </si>
+  <si>
+    <t>input_ID_COD</t>
+  </si>
+  <si>
+    <t>//input[@id='ID_COD']</t>
+  </si>
+  <si>
+    <t>//input[@id='ST_NOMNEW']</t>
+  </si>
+  <si>
+    <t>//input[@id='ST_PRENEW']</t>
+  </si>
+  <si>
+    <t>//button[@value='Valider']</t>
+  </si>
+  <si>
+    <t>input_ST_PRENEW</t>
+  </si>
+  <si>
+    <t>input_ST_NOMNEW</t>
   </si>
 </sst>
 </file>
@@ -1266,7 +1302,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1393,6 +1429,12 @@
         <bgColor rgb="FFFDE39B"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFDE39B"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1428,7 +1470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1612,12 +1654,6 @@
     <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1627,7 +1663,6 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1644,6 +1679,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4965,13 +5009,14 @@
   </sheetPr>
   <dimension ref="A1:BE18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:BE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="32.88671875" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" customWidth="1"/>
     <col min="5" max="5" width="20.88671875" customWidth="1"/>
@@ -5282,10 +5327,10 @@
       <c r="AS3" s="34"/>
       <c r="AT3" s="34"/>
       <c r="AU3" s="34"/>
-      <c r="AV3" s="101" t="s">
+      <c r="AV3" s="100" t="s">
         <v>166</v>
       </c>
-      <c r="AW3" s="102"/>
+      <c r="AW3" s="101"/>
       <c r="AX3" s="34"/>
       <c r="AY3" s="34"/>
       <c r="AZ3" s="34"/>
@@ -5519,7 +5564,7 @@
       <c r="E6" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="F6" s="100" t="s">
+      <c r="F6" s="97" t="s">
         <v>175</v>
       </c>
       <c r="G6" s="44" t="s">
@@ -7190,25 +7235,25 @@
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
-      <c r="D5" s="101" t="s">
+      <c r="D5" s="100" t="s">
         <v>258</v>
       </c>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
       <c r="H5" s="38" t="s">
         <v>259</v>
       </c>
       <c r="I5" s="35" t="s">
         <v>260</v>
       </c>
-      <c r="J5" s="101" t="s">
+      <c r="J5" s="100" t="s">
         <v>261</v>
       </c>
-      <c r="K5" s="102"/>
-      <c r="L5" s="102"/>
-      <c r="M5" s="102"/>
-      <c r="N5" s="102"/>
+      <c r="K5" s="101"/>
+      <c r="L5" s="101"/>
+      <c r="M5" s="101"/>
+      <c r="N5" s="101"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="39" t="s">
@@ -7564,15 +7609,18 @@
   </sheetPr>
   <dimension ref="A1:BB6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.77734375" customWidth="1"/>
     <col min="3" max="3" width="23.44140625" customWidth="1"/>
     <col min="4" max="4" width="25.33203125" customWidth="1"/>
     <col min="5" max="5" width="30.88671875" customWidth="1"/>
+    <col min="35" max="35" width="12.5546875" customWidth="1"/>
     <col min="47" max="47" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7747,251 +7795,325 @@
       <c r="B2" s="83" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="83" t="s">
+      <c r="C2" s="98"/>
+      <c r="D2" s="98" t="s">
         <v>160</v>
       </c>
-      <c r="E2" s="83" t="s">
+      <c r="E2" s="98" t="s">
         <v>160</v>
       </c>
-      <c r="F2" s="83" t="s">
+      <c r="F2" s="98" t="s">
         <v>161</v>
       </c>
-      <c r="G2" s="83" t="s">
+      <c r="G2" s="98" t="s">
         <v>162</v>
       </c>
-      <c r="H2" s="83"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="84"/>
-      <c r="R2" s="84"/>
-      <c r="S2" s="84"/>
-      <c r="T2" s="84"/>
-      <c r="U2" s="84"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="84"/>
-      <c r="X2" s="85" t="s">
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98" t="s">
+        <v>160</v>
+      </c>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="98"/>
+      <c r="S2" s="98"/>
+      <c r="T2" s="98"/>
+      <c r="U2" s="98"/>
+      <c r="V2" s="98"/>
+      <c r="W2" s="98"/>
+      <c r="X2" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="Y2" s="84"/>
-      <c r="Z2" s="84"/>
-      <c r="AA2" s="84"/>
-      <c r="AB2" s="84"/>
-      <c r="AC2" s="84"/>
-      <c r="AD2" s="84"/>
-      <c r="AE2" s="84"/>
-      <c r="AF2" s="84"/>
-      <c r="AG2" s="84"/>
-      <c r="AH2" s="84"/>
-      <c r="AI2" s="84"/>
-      <c r="AJ2" s="84"/>
-      <c r="AK2" s="84"/>
-      <c r="AL2" s="84"/>
-      <c r="AM2" s="84"/>
-      <c r="AN2" s="84"/>
-      <c r="AO2" s="84"/>
-      <c r="AP2" s="85" t="s">
+      <c r="Y2" s="98"/>
+      <c r="Z2" s="98"/>
+      <c r="AA2" s="98"/>
+      <c r="AB2" s="98"/>
+      <c r="AC2" s="98"/>
+      <c r="AD2" s="98"/>
+      <c r="AE2" s="98"/>
+      <c r="AF2" s="98"/>
+      <c r="AG2" s="98"/>
+      <c r="AH2" s="98"/>
+      <c r="AI2" s="98"/>
+      <c r="AJ2" s="98"/>
+      <c r="AK2" s="98"/>
+      <c r="AL2" s="98"/>
+      <c r="AM2" s="98"/>
+      <c r="AN2" s="98"/>
+      <c r="AO2" s="98"/>
+      <c r="AP2" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="AQ2" s="84"/>
-      <c r="AR2" s="84"/>
-      <c r="AS2" s="84"/>
-      <c r="AT2" s="84"/>
-      <c r="AU2" s="83" t="s">
+      <c r="AQ2" s="98"/>
+      <c r="AR2" s="98"/>
+      <c r="AS2" s="98"/>
+      <c r="AT2" s="98"/>
+      <c r="AU2" s="98" t="s">
         <v>160</v>
       </c>
-      <c r="AV2" s="83"/>
-      <c r="AW2" s="84"/>
-      <c r="AX2" s="84"/>
-      <c r="AY2" s="84"/>
-      <c r="AZ2" s="84"/>
-      <c r="BA2" s="84"/>
-      <c r="BB2" s="84"/>
+      <c r="AV2" s="98"/>
+      <c r="AW2" s="98"/>
+      <c r="AX2" s="98"/>
+      <c r="AY2" s="98"/>
+      <c r="AZ2" s="98"/>
+      <c r="BA2" s="98"/>
+      <c r="BB2" s="98"/>
     </row>
     <row r="3" spans="1:54">
       <c r="A3" s="82" t="s">
         <v>164</v>
       </c>
       <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="83" t="s">
+      <c r="C3" s="98"/>
+      <c r="D3" s="98" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="84"/>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="84"/>
-      <c r="S3" s="84"/>
-      <c r="T3" s="84"/>
-      <c r="U3" s="84"/>
-      <c r="V3" s="84"/>
-      <c r="W3" s="84"/>
-      <c r="X3" s="86"/>
-      <c r="Y3" s="84"/>
-      <c r="Z3" s="84"/>
-      <c r="AA3" s="84"/>
-      <c r="AB3" s="84"/>
-      <c r="AC3" s="84"/>
-      <c r="AD3" s="84"/>
-      <c r="AE3" s="84"/>
-      <c r="AF3" s="84"/>
-      <c r="AG3" s="84"/>
-      <c r="AH3" s="84"/>
-      <c r="AI3" s="84"/>
-      <c r="AJ3" s="84"/>
-      <c r="AK3" s="84"/>
-      <c r="AL3" s="84"/>
-      <c r="AM3" s="84"/>
-      <c r="AN3" s="84"/>
-      <c r="AO3" s="84"/>
-      <c r="AP3" s="86"/>
-      <c r="AQ3" s="84"/>
-      <c r="AR3" s="84"/>
-      <c r="AS3" s="84"/>
-      <c r="AT3" s="84"/>
-      <c r="AU3" s="84"/>
-      <c r="AV3" s="84"/>
-      <c r="AW3" s="84"/>
-      <c r="AX3" s="84"/>
-      <c r="AY3" s="84"/>
-      <c r="AZ3" s="84"/>
-      <c r="BA3" s="84"/>
-      <c r="BB3" s="84"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="G3" s="98"/>
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
+      <c r="Q3" s="98"/>
+      <c r="R3" s="98"/>
+      <c r="S3" s="98"/>
+      <c r="T3" s="98"/>
+      <c r="U3" s="98"/>
+      <c r="V3" s="98"/>
+      <c r="W3" s="98"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="98"/>
+      <c r="Z3" s="98"/>
+      <c r="AA3" s="98"/>
+      <c r="AB3" s="98"/>
+      <c r="AC3" s="98"/>
+      <c r="AD3" s="98"/>
+      <c r="AE3" s="98"/>
+      <c r="AF3" s="98"/>
+      <c r="AG3" s="98"/>
+      <c r="AH3" s="98"/>
+      <c r="AI3" s="98"/>
+      <c r="AJ3" s="98"/>
+      <c r="AK3" s="98"/>
+      <c r="AL3" s="98"/>
+      <c r="AM3" s="98"/>
+      <c r="AN3" s="98"/>
+      <c r="AO3" s="98"/>
+      <c r="AP3" s="37"/>
+      <c r="AQ3" s="98"/>
+      <c r="AR3" s="98"/>
+      <c r="AS3" s="98"/>
+      <c r="AT3" s="98"/>
+      <c r="AU3" s="98"/>
+      <c r="AV3" s="98"/>
+      <c r="AW3" s="100" t="s">
+        <v>166</v>
+      </c>
+      <c r="AX3" s="101"/>
+      <c r="AY3" s="98"/>
+      <c r="AZ3" s="98"/>
+      <c r="BA3" s="98"/>
+      <c r="BB3" s="98"/>
     </row>
     <row r="4" spans="1:54">
       <c r="A4" s="82" t="s">
         <v>170</v>
       </c>
       <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="84"/>
-      <c r="N4" s="84"/>
-      <c r="O4" s="84"/>
-      <c r="P4" s="84"/>
-      <c r="Q4" s="84"/>
-      <c r="R4" s="84"/>
-      <c r="S4" s="84"/>
-      <c r="T4" s="84"/>
-      <c r="U4" s="84"/>
-      <c r="V4" s="84"/>
-      <c r="W4" s="84"/>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="84"/>
-      <c r="Z4" s="84"/>
-      <c r="AA4" s="84"/>
-      <c r="AB4" s="84"/>
-      <c r="AC4" s="84"/>
-      <c r="AD4" s="84"/>
-      <c r="AE4" s="84"/>
-      <c r="AF4" s="84"/>
-      <c r="AG4" s="84"/>
-      <c r="AH4" s="84"/>
-      <c r="AI4" s="84"/>
-      <c r="AJ4" s="84"/>
-      <c r="AK4" s="84"/>
-      <c r="AL4" s="84"/>
-      <c r="AM4" s="84"/>
-      <c r="AN4" s="84"/>
-      <c r="AO4" s="84"/>
-      <c r="AP4" s="86"/>
-      <c r="AQ4" s="84"/>
-      <c r="AR4" s="84"/>
-      <c r="AS4" s="84"/>
-      <c r="AT4" s="84"/>
-      <c r="AU4" s="84"/>
-      <c r="AV4" s="84"/>
-      <c r="AW4" s="84"/>
-      <c r="AX4" s="84"/>
-      <c r="AY4" s="84"/>
-      <c r="AZ4" s="84"/>
-      <c r="BA4" s="84"/>
-      <c r="BB4" s="84"/>
+      <c r="C4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="G4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="J4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="K4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="L4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="M4" s="98"/>
+      <c r="N4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="O4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="P4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="R4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="S4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="T4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="U4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="V4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="W4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="98"/>
+      <c r="Z4" s="98"/>
+      <c r="AA4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB4" s="98"/>
+      <c r="AC4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="AD4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="AE4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="AF4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="AH4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI4" s="98"/>
+      <c r="AJ4" s="98"/>
+      <c r="AK4" s="98"/>
+      <c r="AL4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="AM4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="AN4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO4" s="98"/>
+      <c r="AP4" s="37"/>
+      <c r="AQ4" s="98"/>
+      <c r="AR4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="AS4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="AT4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="AU4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="AV4" s="98" t="s">
+        <v>171</v>
+      </c>
+      <c r="AW4" s="98" t="s">
+        <v>172</v>
+      </c>
+      <c r="AX4" s="98" t="s">
+        <v>173</v>
+      </c>
+      <c r="AY4" s="98"/>
+      <c r="AZ4" s="98"/>
+      <c r="BA4" s="98"/>
+      <c r="BB4" s="98"/>
     </row>
     <row r="5" spans="1:54">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="85" t="s">
         <v>174</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="88"/>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="88"/>
-      <c r="R5" s="88"/>
-      <c r="S5" s="88"/>
-      <c r="T5" s="88"/>
-      <c r="U5" s="88"/>
-      <c r="V5" s="88"/>
-      <c r="W5" s="88"/>
-      <c r="X5" s="89"/>
-      <c r="Y5" s="88"/>
-      <c r="Z5" s="88"/>
-      <c r="AA5" s="88"/>
-      <c r="AB5" s="88"/>
-      <c r="AC5" s="88"/>
-      <c r="AD5" s="88"/>
-      <c r="AE5" s="88"/>
-      <c r="AF5" s="88"/>
-      <c r="AG5" s="88"/>
-      <c r="AH5" s="88"/>
-      <c r="AI5" s="88"/>
-      <c r="AJ5" s="88"/>
-      <c r="AK5" s="88"/>
-      <c r="AL5" s="88"/>
-      <c r="AM5" s="88"/>
-      <c r="AN5" s="88"/>
-      <c r="AO5" s="88"/>
-      <c r="AP5" s="89"/>
-      <c r="AQ5" s="88"/>
-      <c r="AR5" s="88"/>
-      <c r="AS5" s="88"/>
-      <c r="AT5" s="88"/>
-      <c r="AU5" s="88"/>
-      <c r="AV5" s="88"/>
-      <c r="AW5" s="88"/>
-      <c r="AX5" s="88"/>
-      <c r="AY5" s="88"/>
-      <c r="AZ5" s="88"/>
-      <c r="BA5" s="88"/>
-      <c r="BB5" s="88"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="86"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="86"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="86"/>
+      <c r="T5" s="86"/>
+      <c r="U5" s="86"/>
+      <c r="V5" s="86"/>
+      <c r="W5" s="86"/>
+      <c r="X5" s="87"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="86"/>
+      <c r="AA5" s="86"/>
+      <c r="AB5" s="86"/>
+      <c r="AC5" s="86"/>
+      <c r="AD5" s="86"/>
+      <c r="AE5" s="86"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="86"/>
+      <c r="AH5" s="86"/>
+      <c r="AI5" s="86"/>
+      <c r="AJ5" s="86"/>
+      <c r="AK5" s="86"/>
+      <c r="AL5" s="86"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="86"/>
+      <c r="AO5" s="86"/>
+      <c r="AP5" s="87"/>
+      <c r="AQ5" s="86"/>
+      <c r="AR5" s="86"/>
+      <c r="AS5" s="86"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="86"/>
+      <c r="AV5" s="86"/>
+      <c r="AW5" s="86"/>
+      <c r="AX5" s="86"/>
+      <c r="AY5" s="86"/>
+      <c r="AZ5" s="86"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="86"/>
     </row>
     <row r="6" spans="1:54">
-      <c r="A6" s="90" t="s">
+      <c r="A6" s="103" t="s">
         <v>276</v>
       </c>
       <c r="B6" s="47" t="s">
@@ -8000,10 +8122,10 @@
       <c r="C6" s="47" t="s">
         <v>276</v>
       </c>
-      <c r="D6" s="91" t="s">
+      <c r="D6" s="88" t="s">
         <v>278</v>
       </c>
-      <c r="E6" s="91" t="s">
+      <c r="E6" s="88" t="s">
         <v>278</v>
       </c>
       <c r="F6" s="47" t="s">
@@ -8012,32 +8134,32 @@
       <c r="G6" s="47" t="s">
         <v>276</v>
       </c>
-      <c r="H6" s="44" t="s">
+      <c r="H6" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="I6" s="47" t="s">
         <v>279</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="J6" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="J6" s="47" t="s">
+      <c r="K6" s="47" t="s">
         <v>281</v>
       </c>
-      <c r="K6" s="47" t="s">
+      <c r="L6" s="89">
+        <v>28</v>
+      </c>
+      <c r="M6" s="90"/>
+      <c r="N6" s="47" t="s">
         <v>282</v>
       </c>
-      <c r="L6" s="92">
-        <v>28</v>
-      </c>
-      <c r="M6" s="93"/>
-      <c r="N6" s="47" t="s">
+      <c r="O6" s="47" t="s">
         <v>283</v>
-      </c>
-      <c r="O6" s="47" t="s">
-        <v>284</v>
       </c>
       <c r="P6" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="Q6" s="92">
+      <c r="Q6" s="89">
         <v>40</v>
       </c>
       <c r="R6" s="47" t="s">
@@ -8055,21 +8177,21 @@
       <c r="V6" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="W6" s="92">
+      <c r="W6" s="89">
         <v>200</v>
       </c>
       <c r="X6" s="59"/>
       <c r="Y6" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="Z6" s="44" t="s">
-        <v>279</v>
+      <c r="Z6" s="58" t="s">
+        <v>177</v>
       </c>
       <c r="AA6" s="47" t="s">
-        <v>285</v>
-      </c>
-      <c r="AB6" s="47" t="s">
-        <v>279</v>
+        <v>284</v>
+      </c>
+      <c r="AB6" s="57" t="s">
+        <v>177</v>
       </c>
       <c r="AC6" s="47" t="s">
         <v>185</v>
@@ -8089,28 +8211,30 @@
       <c r="AH6" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="AI6" s="44" t="s">
+      <c r="AI6" s="58" t="s">
+        <v>186</v>
+      </c>
+      <c r="AJ6" s="58" t="s">
         <v>188</v>
       </c>
-      <c r="AJ6" s="44" t="s">
-        <v>188</v>
-      </c>
-      <c r="AK6" s="44" t="s">
-        <v>188</v>
-      </c>
-      <c r="AL6" s="92">
-        <v>1010128</v>
-      </c>
-      <c r="AM6" s="92">
-        <v>6060628</v>
-      </c>
-      <c r="AN6" s="92">
-        <v>9090928</v>
-      </c>
-      <c r="AO6" s="47" t="s">
-        <v>279</v>
-      </c>
-      <c r="AP6" s="59"/>
+      <c r="AK6" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="AL6" s="102" t="s">
+        <v>367</v>
+      </c>
+      <c r="AM6" s="102" t="s">
+        <v>368</v>
+      </c>
+      <c r="AN6" s="102" t="s">
+        <v>369</v>
+      </c>
+      <c r="AO6" s="57" t="s">
+        <v>177</v>
+      </c>
+      <c r="AP6" s="59" t="s">
+        <v>177</v>
+      </c>
       <c r="AQ6" s="44" t="s">
         <v>185</v>
       </c>
@@ -8123,32 +8247,35 @@
       <c r="AT6" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="AU6" s="91" t="s">
-        <v>286</v>
+      <c r="AU6" s="88" t="s">
+        <v>285</v>
       </c>
       <c r="AV6" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="AW6" s="92">
-        <v>3</v>
+      <c r="AW6" s="89">
+        <v>0</v>
       </c>
       <c r="AX6" s="47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AY6" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="AZ6" s="44" t="s">
-        <v>186</v>
-      </c>
-      <c r="BA6" s="44" t="s">
+      <c r="AZ6" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="BA6" s="58" t="s">
         <v>188</v>
       </c>
-      <c r="BB6" s="44" t="s">
-        <v>188</v>
+      <c r="BB6" s="58" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="AW3:AX3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8158,9 +8285,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -8170,13 +8299,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="B1" s="91" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="94" t="s">
+      <c r="C1" s="91" t="s">
         <v>289</v>
-      </c>
-      <c r="C1" s="94" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -8184,43 +8313,43 @@
         <v>11</v>
       </c>
       <c r="B2" s="42" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2" s="42" t="s">
         <v>291</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="42" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" s="42" t="s">
         <v>293</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="C3" s="42" t="s">
         <v>294</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B4" s="42" t="s">
+        <v>295</v>
+      </c>
+      <c r="C4" s="42" t="s">
         <v>296</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B5" s="42" t="s">
+        <v>297</v>
+      </c>
+      <c r="C5" s="42" t="s">
         <v>298</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -8228,10 +8357,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="42" t="s">
+        <v>299</v>
+      </c>
+      <c r="C6" s="42" t="s">
         <v>300</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -8239,10 +8368,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="42" t="s">
+        <v>301</v>
+      </c>
+      <c r="C7" s="42" t="s">
         <v>302</v>
-      </c>
-      <c r="C7" s="42" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -8250,10 +8379,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="42" t="s">
+        <v>303</v>
+      </c>
+      <c r="C8" s="42" t="s">
         <v>304</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -8261,428 +8390,483 @@
         <v>11</v>
       </c>
       <c r="B9" s="42" t="s">
+        <v>305</v>
+      </c>
+      <c r="C9" s="42" t="s">
         <v>306</v>
       </c>
-      <c r="C9" s="42" t="s">
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="92" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="95" t="s">
+      <c r="B10" s="42" t="s">
         <v>308</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="C10" s="42" t="s">
         <v>309</v>
       </c>
-      <c r="C10" s="42" t="s">
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="92" t="s">
+        <v>307</v>
+      </c>
+      <c r="B11" s="42" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="95" t="s">
-        <v>308</v>
-      </c>
-      <c r="B11" s="42" t="s">
+      <c r="C11" s="42" t="s">
         <v>311</v>
       </c>
-      <c r="C11" s="42" t="s">
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="92" t="s">
+        <v>307</v>
+      </c>
+      <c r="B12" s="42" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="95" t="s">
-        <v>308</v>
-      </c>
-      <c r="B12" s="42" t="s">
+      <c r="C12" s="42" t="s">
         <v>313</v>
       </c>
-      <c r="C12" s="42" t="s">
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="92" t="s">
+        <v>307</v>
+      </c>
+      <c r="B13" s="42" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="95" t="s">
-        <v>308</v>
-      </c>
-      <c r="B13" s="42" t="s">
+      <c r="C13" s="42" t="s">
         <v>315</v>
       </c>
-      <c r="C13" s="42" t="s">
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="92" t="s">
+        <v>307</v>
+      </c>
+      <c r="B14" s="93" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="95" t="s">
-        <v>308</v>
-      </c>
-      <c r="B14" s="96" t="s">
+      <c r="C14" s="93" t="s">
         <v>317</v>
       </c>
-      <c r="C14" s="96" t="s">
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="92" t="s">
+        <v>307</v>
+      </c>
+      <c r="B15" s="93" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="95" t="s">
-        <v>308</v>
-      </c>
-      <c r="B15" s="96" t="s">
+      <c r="C15" s="93" t="s">
         <v>319</v>
       </c>
-      <c r="C15" s="96" t="s">
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="92" t="s">
+        <v>307</v>
+      </c>
+      <c r="B16" s="93" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="95" t="s">
-        <v>308</v>
-      </c>
-      <c r="B16" s="96" t="s">
+      <c r="C16" s="93" t="s">
         <v>321</v>
       </c>
-      <c r="C16" s="96" t="s">
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="94" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="97" t="s">
+      <c r="B17" s="42" t="s">
         <v>323</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="C17" s="42" t="s">
         <v>324</v>
       </c>
-      <c r="C17" s="42" t="s">
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="94" t="s">
+        <v>322</v>
+      </c>
+      <c r="B18" s="42" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="97" t="s">
-        <v>323</v>
-      </c>
-      <c r="B18" s="42" t="s">
+      <c r="C18" s="42" t="s">
         <v>326</v>
       </c>
-      <c r="C18" s="42" t="s">
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="94" t="s">
+        <v>322</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="C19" s="42" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="97" t="s">
-        <v>323</v>
-      </c>
-      <c r="B19" s="42" t="s">
-        <v>313</v>
-      </c>
-      <c r="C19" s="42" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="94" t="s">
+        <v>322</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>314</v>
+      </c>
+      <c r="C20" s="42" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="97" t="s">
-        <v>323</v>
-      </c>
-      <c r="B20" s="42" t="s">
-        <v>315</v>
-      </c>
-      <c r="C20" s="42" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" s="94" t="s">
+        <v>322</v>
+      </c>
+      <c r="B21" s="93" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="97" t="s">
-        <v>323</v>
-      </c>
-      <c r="B21" s="96" t="s">
+      <c r="C21" s="93" t="s">
         <v>330</v>
       </c>
-      <c r="C21" s="96" t="s">
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="94" t="s">
+        <v>322</v>
+      </c>
+      <c r="B22" s="93" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="97" t="s">
-        <v>323</v>
-      </c>
-      <c r="B22" s="96" t="s">
+      <c r="C22" s="93" t="s">
         <v>332</v>
       </c>
-      <c r="C22" s="96" t="s">
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="94" t="s">
+        <v>322</v>
+      </c>
+      <c r="B23" s="93" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="97" t="s">
-        <v>323</v>
-      </c>
-      <c r="B23" s="96" t="s">
+      <c r="C23" s="93" t="s">
         <v>334</v>
       </c>
-      <c r="C23" s="96" t="s">
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="94" t="s">
+        <v>322</v>
+      </c>
+      <c r="B24" s="93" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="97" t="s">
-        <v>323</v>
-      </c>
-      <c r="B24" s="96" t="s">
+      <c r="C24" s="93" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="95" t="s">
         <v>336</v>
       </c>
-      <c r="C24" s="96" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="98" t="s">
+      <c r="B25" s="42" t="s">
         <v>337</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="C25" s="43" t="s">
         <v>338</v>
       </c>
-      <c r="C25" s="43" t="s">
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="95" t="s">
+        <v>336</v>
+      </c>
+      <c r="B26" s="42" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="98" t="s">
-        <v>337</v>
-      </c>
-      <c r="B26" s="42" t="s">
+      <c r="C26" s="47" t="s">
         <v>340</v>
       </c>
-      <c r="C26" s="47" t="s">
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="95" t="s">
+        <v>336</v>
+      </c>
+      <c r="B27" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="C27" s="42" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="98" t="s">
-        <v>337</v>
-      </c>
-      <c r="B27" s="42" t="s">
-        <v>313</v>
-      </c>
-      <c r="C27" s="42" t="s">
+    <row r="28" spans="1:3">
+      <c r="A28" s="95" t="s">
+        <v>336</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>314</v>
+      </c>
+      <c r="C28" s="42" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="98" t="s">
-        <v>337</v>
-      </c>
-      <c r="B28" s="42" t="s">
-        <v>315</v>
-      </c>
-      <c r="C28" s="42" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" s="95" t="s">
+        <v>336</v>
+      </c>
+      <c r="B29" s="47" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="98" t="s">
-        <v>337</v>
-      </c>
-      <c r="B29" s="47" t="s">
+      <c r="C29" s="47" t="s">
         <v>344</v>
       </c>
-      <c r="C29" s="47" t="s">
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="95" t="s">
+        <v>336</v>
+      </c>
+      <c r="B30" s="93" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="98" t="s">
-        <v>337</v>
-      </c>
-      <c r="B30" s="96" t="s">
+      <c r="C30" s="93" t="s">
         <v>346</v>
       </c>
-      <c r="C30" s="96" t="s">
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="95" t="s">
+        <v>336</v>
+      </c>
+      <c r="B31" s="93" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="98" t="s">
-        <v>337</v>
-      </c>
-      <c r="B31" s="96" t="s">
+      <c r="C31" s="93" t="s">
         <v>348</v>
       </c>
-      <c r="C31" s="96" t="s">
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="95" t="s">
+        <v>336</v>
+      </c>
+      <c r="B32" s="93" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="98" t="s">
-        <v>337</v>
-      </c>
-      <c r="B32" s="96" t="s">
+      <c r="C32" s="93" t="s">
         <v>350</v>
       </c>
-      <c r="C32" s="96" t="s">
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="95" t="s">
+        <v>336</v>
+      </c>
+      <c r="B33" s="93" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="98" t="s">
-        <v>337</v>
-      </c>
-      <c r="B33" s="96" t="s">
+      <c r="C33" s="96" t="s">
         <v>352</v>
       </c>
-      <c r="C33" s="99" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="42" t="s">
+    </row>
+    <row r="34" spans="1:3" s="99" customFormat="1">
+      <c r="A34" s="104" t="s">
+        <v>370</v>
+      </c>
+      <c r="B34" s="57" t="s">
+        <v>371</v>
+      </c>
+      <c r="C34" s="97" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="99" customFormat="1">
+      <c r="A35" s="104" t="s">
+        <v>370</v>
+      </c>
+      <c r="B35" s="97" t="s">
+        <v>387</v>
+      </c>
+      <c r="C35" s="97" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="99" customFormat="1">
+      <c r="A36" s="104" t="s">
+        <v>370</v>
+      </c>
+      <c r="B36" s="97" t="s">
+        <v>393</v>
+      </c>
+      <c r="C36" s="97" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="99" customFormat="1">
+      <c r="A37" s="104" t="s">
+        <v>370</v>
+      </c>
+      <c r="B37" s="97" t="s">
+        <v>392</v>
+      </c>
+      <c r="C37" s="97" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="99" customFormat="1">
+      <c r="A38" s="104" t="s">
+        <v>370</v>
+      </c>
+      <c r="B38" s="97" t="s">
         <v>293</v>
       </c>
-      <c r="B34" s="42" t="s">
-        <v>354</v>
-      </c>
-      <c r="C34" s="42" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="42" t="s">
-        <v>293</v>
-      </c>
-      <c r="B35" s="42" t="s">
-        <v>356</v>
-      </c>
-      <c r="C35" s="42" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="42" t="s">
-        <v>293</v>
-      </c>
-      <c r="B36" s="42" t="s">
-        <v>358</v>
-      </c>
-      <c r="C36" s="42" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="42" t="s">
-        <v>293</v>
-      </c>
-      <c r="B37" s="42" t="s">
-        <v>360</v>
-      </c>
-      <c r="C37" s="42" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="42" t="s">
-        <v>293</v>
-      </c>
-      <c r="B38" s="42" t="s">
-        <v>362</v>
-      </c>
-      <c r="C38" s="42" t="s">
-        <v>363</v>
+      <c r="C38" s="97" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="42" t="s">
-        <v>293</v>
-      </c>
-      <c r="B39" s="42" t="s">
-        <v>364</v>
-      </c>
-      <c r="C39" s="42" t="s">
-        <v>365</v>
+        <v>292</v>
+      </c>
+      <c r="B39" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="C39" s="97" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B40" s="42" t="s">
-        <v>366</v>
-      </c>
-      <c r="C40" s="42" t="s">
-        <v>367</v>
+        <v>354</v>
+      </c>
+      <c r="C40" s="57" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B41" s="42" t="s">
-        <v>368</v>
-      </c>
-      <c r="C41" s="42" t="s">
-        <v>369</v>
+        <v>355</v>
+      </c>
+      <c r="C41" s="57" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B42" s="42" t="s">
-        <v>370</v>
-      </c>
-      <c r="C42" s="42" t="s">
-        <v>371</v>
+        <v>356</v>
+      </c>
+      <c r="C42" s="57" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B43" s="42" t="s">
-        <v>372</v>
-      </c>
-      <c r="C43" s="47" t="s">
-        <v>373</v>
+        <v>357</v>
+      </c>
+      <c r="C43" s="57" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B44" s="42" t="s">
-        <v>374</v>
-      </c>
-      <c r="C44" s="42" t="s">
-        <v>375</v>
+        <v>358</v>
+      </c>
+      <c r="C44" s="57" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B45" s="42" t="s">
-        <v>376</v>
-      </c>
-      <c r="C45" s="42" t="s">
-        <v>377</v>
+        <v>359</v>
+      </c>
+      <c r="C45" s="57" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>378</v>
-      </c>
-      <c r="C46" s="42" t="s">
-        <v>379</v>
+        <v>360</v>
+      </c>
+      <c r="C46" s="57" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B47" s="42" t="s">
-        <v>380</v>
-      </c>
-      <c r="C47" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="C47" s="57" t="s">
         <v>381</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="42" t="s">
+        <v>292</v>
+      </c>
+      <c r="B48" s="42" t="s">
+        <v>362</v>
+      </c>
+      <c r="C48" s="57" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="42" t="s">
+        <v>292</v>
+      </c>
+      <c r="B49" s="42" t="s">
+        <v>363</v>
+      </c>
+      <c r="C49" s="57" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="42" t="s">
+        <v>292</v>
+      </c>
+      <c r="B50" s="42" t="s">
+        <v>364</v>
+      </c>
+      <c r="C50" s="57" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="42" t="s">
+        <v>292</v>
+      </c>
+      <c r="B51" s="42" t="s">
+        <v>365</v>
+      </c>
+      <c r="C51" s="57" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="42" t="s">
+        <v>292</v>
+      </c>
+      <c r="B52" s="42" t="s">
+        <v>366</v>
+      </c>
+      <c r="C52" s="57" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Review KW to include JDD as a parameter
Pour simplifier l'écriture du code de test, passer le myJDD et le code
du champs aux fonction KW 
AS IS : KW.scrollAndSetText(myJDD.makeTO('ID_CODINT'),
myJDD.getStrData('ID_CODINT'))
TO BE : KW.scrollAndSetText(myJDD,'ID_CODINT')
	 		 
AS IS : scrollAndSetText(TestObject tObj, String text, int timeOut =
GlobalVariable.TIMEOUT, String status = 'FAIL')
TO BE : scrollAndSetText(my.JDD myJDD, String name, String text, int
timeOut = GlobalVariable.TIMEOUT, String status = 'FAIL')
	
Mofif
		reprise de toutes les definitions de KW
		reprise NAV
		reprise de tous les TC
</commit_message>
<xml_diff>
--- a/TNR_JDD/RO/JDD.RO.ACT.xlsx
+++ b/TNR_JDD/RO/JDD.RO.ACT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="228" yWindow="504" windowWidth="15612" windowHeight="8412" activeTab="2"/>
+    <workbookView xWindow="228" yWindow="504" windowWidth="15612" windowHeight="8412" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="387">
   <si>
     <t>Date</t>
   </si>
@@ -1449,7 +1449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1657,10 +1657,13 @@
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4982,8 +4985,8 @@
   </sheetPr>
   <dimension ref="A1:BE18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AB12" sqref="AB12"/>
+    <sheetView topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:BA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -5299,10 +5302,10 @@
       <c r="AS3" s="34"/>
       <c r="AT3" s="34"/>
       <c r="AU3" s="34"/>
-      <c r="AV3" s="98" t="s">
+      <c r="AV3" s="100" t="s">
         <v>166</v>
       </c>
-      <c r="AW3" s="99"/>
+      <c r="AW3" s="101"/>
       <c r="AX3" s="34"/>
       <c r="AY3" s="34"/>
       <c r="AZ3" s="34"/>
@@ -5357,26 +5360,26 @@
       <c r="N4" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="O4" s="35" t="s">
-        <v>171</v>
+      <c r="O4" s="99" t="s">
+        <v>386</v>
       </c>
       <c r="P4" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="Q4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="R4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="S4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="T4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="U4" s="35" t="s">
-        <v>171</v>
+      <c r="Q4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="R4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="S4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="T4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="U4" s="99" t="s">
+        <v>386</v>
       </c>
       <c r="V4" s="35" t="s">
         <v>171</v>
@@ -5388,23 +5391,23 @@
         <v>171</v>
       </c>
       <c r="AA4" s="34"/>
-      <c r="AB4" s="100" t="s">
+      <c r="AB4" s="99" t="s">
         <v>386</v>
       </c>
-      <c r="AC4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AD4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AE4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AF4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AG4" s="35" t="s">
-        <v>171</v>
+      <c r="AC4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AD4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AE4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AF4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AG4" s="99" t="s">
+        <v>386</v>
       </c>
       <c r="AH4" s="34"/>
       <c r="AI4" s="34"/>
@@ -5420,21 +5423,23 @@
       </c>
       <c r="AN4" s="34"/>
       <c r="AO4" s="37"/>
-      <c r="AP4" s="34"/>
-      <c r="AQ4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AR4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AS4" s="35" t="s">
-        <v>171</v>
+      <c r="AP4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AQ4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AR4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AS4" s="99" t="s">
+        <v>386</v>
       </c>
       <c r="AT4" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="AU4" s="35" t="s">
-        <v>171</v>
+      <c r="AU4" s="99" t="s">
+        <v>386</v>
       </c>
       <c r="AV4" s="35" t="s">
         <v>172</v>
@@ -7207,25 +7212,25 @@
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
-      <c r="D5" s="98" t="s">
+      <c r="D5" s="100" t="s">
         <v>258</v>
       </c>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
       <c r="H5" s="38" t="s">
         <v>259</v>
       </c>
       <c r="I5" s="35" t="s">
         <v>260</v>
       </c>
-      <c r="J5" s="98" t="s">
+      <c r="J5" s="100" t="s">
         <v>261</v>
       </c>
-      <c r="K5" s="99"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="99"/>
-      <c r="N5" s="99"/>
+      <c r="K5" s="101"/>
+      <c r="L5" s="101"/>
+      <c r="M5" s="101"/>
+      <c r="N5" s="101"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="39" t="s">
@@ -7581,7 +7586,9 @@
   </sheetPr>
   <dimension ref="A1:BC6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AX18" sqref="AX18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -7930,10 +7937,10 @@
       <c r="AT3" s="34"/>
       <c r="AU3" s="34"/>
       <c r="AV3" s="34"/>
-      <c r="AW3" s="98" t="s">
+      <c r="AW3" s="100" t="s">
         <v>166</v>
       </c>
-      <c r="AX3" s="99"/>
+      <c r="AX3" s="101"/>
       <c r="AY3" s="34"/>
       <c r="AZ3" s="34"/>
       <c r="BA3" s="34"/>
@@ -7945,128 +7952,130 @@
         <v>170</v>
       </c>
       <c r="B4" s="84"/>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="35" t="s">
+      <c r="D4" s="98"/>
+      <c r="E4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="H4" s="34"/>
-      <c r="I4" s="35" t="s">
+      <c r="H4" s="98"/>
+      <c r="I4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="J4" s="35" t="s">
+      <c r="J4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="K4" s="35" t="s">
+      <c r="K4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="L4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="M4" s="34"/>
-      <c r="N4" s="35" t="s">
+      <c r="M4" s="98"/>
+      <c r="N4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="O4" s="35" t="s">
+      <c r="O4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="P4" s="35" t="s">
+      <c r="P4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="Q4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="Q4" s="35" t="s">
+      <c r="R4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="S4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="T4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="U4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="V4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="W4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="R4" s="35" t="s">
+      <c r="X4" s="37"/>
+      <c r="Y4" s="98"/>
+      <c r="Z4" s="98"/>
+      <c r="AA4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="S4" s="35" t="s">
+      <c r="AB4" s="98"/>
+      <c r="AC4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AD4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AE4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AF4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AG4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AH4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AI4" s="98"/>
+      <c r="AJ4" s="98"/>
+      <c r="AK4" s="98"/>
+      <c r="AL4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="T4" s="35" t="s">
+      <c r="AM4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="U4" s="35" t="s">
+      <c r="AN4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="V4" s="35" t="s">
+      <c r="AO4" s="98"/>
+      <c r="AP4" s="37"/>
+      <c r="AQ4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AR4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AS4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AT4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AU4" s="98" t="s">
         <v>171</v>
       </c>
-      <c r="W4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="X4" s="37"/>
-      <c r="Y4" s="34"/>
-      <c r="Z4" s="34"/>
-      <c r="AA4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AD4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AE4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AF4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AG4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AH4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AI4" s="34"/>
-      <c r="AJ4" s="34"/>
-      <c r="AK4" s="34"/>
-      <c r="AL4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AM4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AN4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AO4" s="34"/>
-      <c r="AP4" s="37"/>
-      <c r="AQ4" s="34"/>
-      <c r="AR4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AS4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AT4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AU4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AV4" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AW4" s="35" t="s">
+      <c r="AV4" s="99" t="s">
+        <v>386</v>
+      </c>
+      <c r="AW4" s="98" t="s">
         <v>172</v>
       </c>
-      <c r="AX4" s="35" t="s">
+      <c r="AX4" s="98" t="s">
         <v>173</v>
       </c>
-      <c r="AY4" s="34"/>
-      <c r="AZ4" s="34"/>
-      <c r="BA4" s="34"/>
-      <c r="BB4" s="34"/>
+      <c r="AY4" s="98"/>
+      <c r="AZ4" s="98"/>
+      <c r="BA4" s="98"/>
+      <c r="BB4" s="98"/>
       <c r="BC4" s="34"/>
     </row>
     <row r="5" spans="1:55">

</xml_diff>

<commit_message>
Ajout d'un fichier log DEBUG séparé
</commit_message>
<xml_diff>
--- a/TNR_JDD/RO/JDD.RO.ACT.xlsx
+++ b/TNR_JDD/RO/JDD.RO.ACT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="228" yWindow="504" windowWidth="15612" windowHeight="8412" activeTab="6"/>
+    <workbookView xWindow="228" yWindow="504" windowWidth="15612" windowHeight="8412" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
@@ -1462,7 +1462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1677,6 +1677,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4998,8 +5001,8 @@
   </sheetPr>
   <dimension ref="A1:BE18"/>
   <sheetViews>
-    <sheetView topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:BA4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AS31" sqref="AS30:AS31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -7599,8 +7602,8 @@
   </sheetPr>
   <dimension ref="A1:BB6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:BB4"/>
+    <sheetView topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="AW3" sqref="AW3:AX3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -7948,7 +7951,7 @@
       <c r="AT3" s="34"/>
       <c r="AU3" s="34"/>
       <c r="AV3" s="34"/>
-      <c r="AW3" s="100" t="s">
+      <c r="AW3" s="102" t="s">
         <v>166</v>
       </c>
       <c r="AX3" s="101"/>

</xml_diff>

<commit_message>
Clean (my.Log) import my.Log as MYLOG and replace all my.log by MYLOG
</commit_message>
<xml_diff>
--- a/TNR_JDD/RO/JDD.RO.ACT.xlsx
+++ b/TNR_JDD/RO/JDD.RO.ACT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="624" windowWidth="18108" windowHeight="8148" activeTab="2"/>
+    <workbookView xWindow="516" yWindow="624" windowWidth="18108" windowHeight="8148" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="387">
   <si>
     <t>Date</t>
   </si>
@@ -853,9 +853,6 @@
     <t>RO.ACT.004EMP.SRL.01..........</t>
   </si>
   <si>
-    <t>SOURCE</t>
-  </si>
-  <si>
     <t>RO.ACT.005.FON.01</t>
   </si>
   <si>
@@ -1187,6 +1184,9 @@
   </si>
   <si>
     <t>ST_DES*CAL*ID_CODCAL</t>
+  </si>
+  <si>
+    <t>ID_CODINT_SRC</t>
   </si>
 </sst>
 </file>
@@ -1627,9 +1627,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1671,6 +1668,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4992,15 +4992,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BE18"/>
+  <dimension ref="A1:BE17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="BE4" sqref="BE4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.88671875" customWidth="1"/>
     <col min="4" max="4" width="24.6640625" customWidth="1"/>
     <col min="5" max="5" width="20.88671875" customWidth="1"/>
@@ -5016,7 +5017,7 @@
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="99" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="28" t="s">
@@ -5189,7 +5190,9 @@
       <c r="A2" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="B2" s="34"/>
+      <c r="B2" s="65" t="s">
+        <v>219</v>
+      </c>
       <c r="C2" s="35" t="s">
         <v>160</v>
       </c>
@@ -5223,7 +5226,7 @@
       <c r="W2" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="X2" s="101"/>
+      <c r="X2" s="100"/>
       <c r="Y2" s="34"/>
       <c r="Z2" s="34"/>
       <c r="AA2" s="34"/>
@@ -5314,10 +5317,10 @@
       <c r="AS3" s="34"/>
       <c r="AT3" s="34"/>
       <c r="AU3" s="34"/>
-      <c r="AV3" s="103" t="s">
+      <c r="AV3" s="102" t="s">
         <v>166</v>
       </c>
-      <c r="AW3" s="104"/>
+      <c r="AW3" s="103"/>
       <c r="AX3" s="34"/>
       <c r="AY3" s="34"/>
       <c r="AZ3" s="34"/>
@@ -5331,8 +5334,8 @@
       <c r="BD3" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="BE3" s="101" t="s">
-        <v>386</v>
+      <c r="BE3" s="100" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:57" ht="13.2">
@@ -5418,10 +5421,10 @@
       <c r="AF4" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="AG4" s="103" t="s">
+      <c r="AG4" s="102" t="s">
         <v>171</v>
       </c>
-      <c r="AH4" s="104"/>
+      <c r="AH4" s="103"/>
       <c r="AI4" s="39"/>
       <c r="AJ4" s="39"/>
       <c r="AK4" s="38" t="s">
@@ -6579,65 +6582,6 @@
       <c r="BD17" s="62"/>
       <c r="BE17" s="62"/>
     </row>
-    <row r="18" spans="1:57" ht="13.2">
-      <c r="A18" s="58"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="59"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="59"/>
-      <c r="R18" s="59"/>
-      <c r="S18" s="59"/>
-      <c r="T18" s="59"/>
-      <c r="U18" s="59"/>
-      <c r="V18" s="59"/>
-      <c r="W18" s="61"/>
-      <c r="X18" s="60"/>
-      <c r="Y18" s="60"/>
-      <c r="Z18" s="59"/>
-      <c r="AA18" s="59"/>
-      <c r="AB18" s="59"/>
-      <c r="AC18" s="59"/>
-      <c r="AD18" s="59"/>
-      <c r="AE18" s="59"/>
-      <c r="AF18" s="59"/>
-      <c r="AG18" s="59"/>
-      <c r="AH18" s="60"/>
-      <c r="AI18" s="60"/>
-      <c r="AJ18" s="60"/>
-      <c r="AK18" s="59"/>
-      <c r="AL18" s="59"/>
-      <c r="AM18" s="59"/>
-      <c r="AN18" s="59"/>
-      <c r="AO18" s="61"/>
-      <c r="AP18" s="60"/>
-      <c r="AQ18" s="60"/>
-      <c r="AR18" s="60"/>
-      <c r="AS18" s="60"/>
-      <c r="AT18" s="59"/>
-      <c r="AU18" s="59"/>
-      <c r="AV18" s="59"/>
-      <c r="AW18" s="59"/>
-      <c r="AX18" s="60"/>
-      <c r="AY18" s="60"/>
-      <c r="AZ18" s="60"/>
-      <c r="BA18" s="60"/>
-      <c r="BB18" s="62"/>
-      <c r="BC18" s="62"/>
-      <c r="BD18" s="62"/>
-      <c r="BE18" s="62"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="AV3:AW3"/>
@@ -6659,7 +6603,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20.21875" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="4" max="4" width="22.44140625" customWidth="1"/>
     <col min="5" max="5" width="20.44140625" customWidth="1"/>
@@ -6667,7 +6611,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="77" t="s">
         <v>122</v>
       </c>
       <c r="B1" s="28" t="s">
@@ -7225,12 +7169,12 @@
       </c>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
-      <c r="D5" s="103" t="s">
+      <c r="D5" s="102" t="s">
         <v>258</v>
       </c>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
-      <c r="G5" s="104"/>
+      <c r="E5" s="103"/>
+      <c r="F5" s="103"/>
+      <c r="G5" s="103"/>
       <c r="H5" s="38" t="s">
         <v>259</v>
       </c>
@@ -7598,8 +7542,8 @@
   </sheetPr>
   <dimension ref="A1:BB6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AX9" sqref="AX9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -7650,14 +7594,15 @@
     <col min="48" max="48" width="10.88671875" customWidth="1"/>
     <col min="49" max="49" width="7.6640625" customWidth="1"/>
     <col min="50" max="51" width="13.6640625" customWidth="1"/>
-    <col min="52" max="54" width="13.44140625" customWidth="1"/>
+    <col min="52" max="53" width="13.44140625" customWidth="1"/>
+    <col min="54" max="54" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54">
       <c r="A1" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="99" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="79" t="s">
@@ -7813,12 +7758,12 @@
       <c r="BA1" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="BB1" s="83" t="s">
-        <v>275</v>
+      <c r="BB1" s="104" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:54">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="83" t="s">
         <v>159</v>
       </c>
       <c r="B2" s="34"/>
@@ -7889,12 +7834,12 @@
       <c r="AY2" s="34"/>
       <c r="AZ2" s="34"/>
       <c r="BA2" s="34"/>
-      <c r="BB2" s="85" t="s">
+      <c r="BB2" s="84" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:54">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="83" t="s">
         <v>164</v>
       </c>
       <c r="B3" s="34"/>
@@ -7945,18 +7890,18 @@
       <c r="AS3" s="34"/>
       <c r="AT3" s="34"/>
       <c r="AU3" s="34"/>
-      <c r="AV3" s="103" t="s">
+      <c r="AV3" s="102" t="s">
         <v>166</v>
       </c>
-      <c r="AW3" s="104"/>
+      <c r="AW3" s="103"/>
       <c r="AX3" s="34"/>
       <c r="AY3" s="34"/>
       <c r="AZ3" s="34"/>
       <c r="BA3" s="34"/>
-      <c r="BB3" s="86"/>
+      <c r="BB3" s="85"/>
     </row>
     <row r="4" spans="1:54">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="83" t="s">
         <v>169</v>
       </c>
       <c r="B4" s="38" t="s">
@@ -8038,10 +7983,10 @@
       <c r="AF4" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="AG4" s="103" t="s">
+      <c r="AG4" s="102" t="s">
         <v>171</v>
       </c>
-      <c r="AH4" s="104"/>
+      <c r="AH4" s="103"/>
       <c r="AI4" s="39"/>
       <c r="AJ4" s="39"/>
       <c r="AK4" s="38" t="s">
@@ -8083,108 +8028,108 @@
       <c r="AY4" s="39"/>
       <c r="AZ4" s="39"/>
       <c r="BA4" s="39"/>
-      <c r="BB4" s="86"/>
+      <c r="BB4" s="85"/>
     </row>
     <row r="5" spans="1:54">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="86" t="s">
         <v>174</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="88"/>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="88"/>
-      <c r="R5" s="88"/>
-      <c r="S5" s="88"/>
-      <c r="T5" s="88"/>
-      <c r="U5" s="88"/>
-      <c r="V5" s="88"/>
-      <c r="W5" s="89"/>
-      <c r="X5" s="88"/>
-      <c r="Y5" s="88"/>
-      <c r="Z5" s="88"/>
-      <c r="AA5" s="88"/>
-      <c r="AB5" s="88"/>
-      <c r="AC5" s="88"/>
-      <c r="AD5" s="88"/>
-      <c r="AE5" s="88"/>
-      <c r="AF5" s="88"/>
-      <c r="AG5" s="88"/>
-      <c r="AH5" s="88"/>
-      <c r="AI5" s="88"/>
-      <c r="AJ5" s="88"/>
-      <c r="AK5" s="88"/>
-      <c r="AL5" s="88"/>
-      <c r="AM5" s="88"/>
-      <c r="AN5" s="88"/>
-      <c r="AO5" s="89"/>
-      <c r="AP5" s="88"/>
-      <c r="AQ5" s="88"/>
-      <c r="AR5" s="88"/>
-      <c r="AS5" s="88"/>
-      <c r="AT5" s="88"/>
-      <c r="AU5" s="88"/>
-      <c r="AV5" s="88"/>
-      <c r="AW5" s="88"/>
-      <c r="AX5" s="88"/>
-      <c r="AY5" s="88"/>
-      <c r="AZ5" s="88"/>
-      <c r="BA5" s="88"/>
-      <c r="BB5" s="88"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
+      <c r="L5" s="87"/>
+      <c r="M5" s="87"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="87"/>
+      <c r="Q5" s="87"/>
+      <c r="R5" s="87"/>
+      <c r="S5" s="87"/>
+      <c r="T5" s="87"/>
+      <c r="U5" s="87"/>
+      <c r="V5" s="87"/>
+      <c r="W5" s="88"/>
+      <c r="X5" s="87"/>
+      <c r="Y5" s="87"/>
+      <c r="Z5" s="87"/>
+      <c r="AA5" s="87"/>
+      <c r="AB5" s="87"/>
+      <c r="AC5" s="87"/>
+      <c r="AD5" s="87"/>
+      <c r="AE5" s="87"/>
+      <c r="AF5" s="87"/>
+      <c r="AG5" s="87"/>
+      <c r="AH5" s="87"/>
+      <c r="AI5" s="87"/>
+      <c r="AJ5" s="87"/>
+      <c r="AK5" s="87"/>
+      <c r="AL5" s="87"/>
+      <c r="AM5" s="87"/>
+      <c r="AN5" s="87"/>
+      <c r="AO5" s="88"/>
+      <c r="AP5" s="87"/>
+      <c r="AQ5" s="87"/>
+      <c r="AR5" s="87"/>
+      <c r="AS5" s="87"/>
+      <c r="AT5" s="87"/>
+      <c r="AU5" s="87"/>
+      <c r="AV5" s="87"/>
+      <c r="AW5" s="87"/>
+      <c r="AX5" s="87"/>
+      <c r="AY5" s="87"/>
+      <c r="AZ5" s="87"/>
+      <c r="BA5" s="87"/>
+      <c r="BB5" s="87"/>
     </row>
     <row r="6" spans="1:54">
       <c r="A6" s="43" t="s">
+        <v>275</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="C6" s="44" t="s">
         <v>276</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="D6" s="44" t="s">
         <v>276</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="E6" s="44" t="s">
         <v>277</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="F6" s="44" t="s">
         <v>277</v>
-      </c>
-      <c r="E6" s="44" t="s">
-        <v>278</v>
-      </c>
-      <c r="F6" s="44" t="s">
-        <v>278</v>
       </c>
       <c r="G6" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="H6" s="90" t="s">
+      <c r="H6" s="89" t="s">
+        <v>278</v>
+      </c>
+      <c r="I6" s="89" t="s">
         <v>279</v>
       </c>
-      <c r="I6" s="90" t="s">
+      <c r="J6" s="44" t="s">
         <v>280</v>
       </c>
-      <c r="J6" s="44" t="s">
+      <c r="K6" s="89" t="s">
+        <v>177</v>
+      </c>
+      <c r="L6" s="90" t="s">
         <v>281</v>
       </c>
-      <c r="K6" s="90" t="s">
-        <v>177</v>
-      </c>
-      <c r="L6" s="91" t="s">
+      <c r="M6" s="44" t="s">
         <v>282</v>
       </c>
-      <c r="M6" s="44" t="s">
+      <c r="N6" s="44" t="s">
         <v>283</v>
-      </c>
-      <c r="N6" s="44" t="s">
-        <v>284</v>
       </c>
       <c r="O6" s="44" t="s">
         <v>185</v>
@@ -8210,7 +8155,7 @@
       <c r="V6" s="47">
         <v>100</v>
       </c>
-      <c r="W6" s="92" t="s">
+      <c r="W6" s="91" t="s">
         <v>177</v>
       </c>
       <c r="X6" s="45" t="s">
@@ -8220,7 +8165,7 @@
         <v>177</v>
       </c>
       <c r="Z6" s="44" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AA6" s="44" t="s">
         <v>177</v>
@@ -8252,14 +8197,14 @@
       <c r="AJ6" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="AK6" s="93" t="s">
+      <c r="AK6" s="92" t="s">
+        <v>285</v>
+      </c>
+      <c r="AL6" s="92" t="s">
         <v>286</v>
       </c>
-      <c r="AL6" s="93" t="s">
+      <c r="AM6" s="92" t="s">
         <v>287</v>
-      </c>
-      <c r="AM6" s="93" t="s">
-        <v>288</v>
       </c>
       <c r="AN6" s="44" t="s">
         <v>177</v>
@@ -8280,7 +8225,7 @@
         <v>185</v>
       </c>
       <c r="AT6" s="44" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AU6" s="44" t="s">
         <v>185</v>
@@ -8303,8 +8248,8 @@
       <c r="BA6" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="BB6" s="90" t="s">
-        <v>278</v>
+      <c r="BB6" s="89" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -8335,46 +8280,46 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="B1" s="93" t="s">
         <v>289</v>
       </c>
-      <c r="B1" s="94" t="s">
+      <c r="C1" s="93" t="s">
         <v>290</v>
-      </c>
-      <c r="C1" s="94" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="44" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>292</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="C2" s="44" t="s">
         <v>293</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B3" s="44" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3" s="44" t="s">
         <v>295</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B4" s="44" t="s">
+        <v>296</v>
+      </c>
+      <c r="C4" s="44" t="s">
         <v>297</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -8382,10 +8327,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="44" t="s">
+        <v>298</v>
+      </c>
+      <c r="C5" s="44" t="s">
         <v>299</v>
-      </c>
-      <c r="C5" s="44" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -8393,472 +8338,472 @@
         <v>11</v>
       </c>
       <c r="B6" s="44" t="s">
+        <v>300</v>
+      </c>
+      <c r="C6" s="44" t="s">
         <v>301</v>
       </c>
-      <c r="C6" s="44" t="s">
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="94" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="95" t="s">
+      <c r="B7" s="44" t="s">
         <v>303</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="C7" s="44" t="s">
         <v>304</v>
       </c>
-      <c r="C7" s="44" t="s">
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="94" t="s">
+        <v>302</v>
+      </c>
+      <c r="B8" s="44" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="95" t="s">
-        <v>303</v>
-      </c>
-      <c r="B8" s="44" t="s">
+      <c r="C8" s="44" t="s">
         <v>306</v>
       </c>
-      <c r="C8" s="44" t="s">
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="94" t="s">
+        <v>302</v>
+      </c>
+      <c r="B9" s="44" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="95" t="s">
-        <v>303</v>
-      </c>
-      <c r="B9" s="44" t="s">
+      <c r="C9" s="44" t="s">
         <v>308</v>
       </c>
-      <c r="C9" s="44" t="s">
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="94" t="s">
+        <v>302</v>
+      </c>
+      <c r="B10" s="44" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="95" t="s">
-        <v>303</v>
-      </c>
-      <c r="B10" s="44" t="s">
+      <c r="C10" s="44" t="s">
         <v>310</v>
       </c>
-      <c r="C10" s="44" t="s">
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="94" t="s">
+        <v>302</v>
+      </c>
+      <c r="B11" s="95" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="95" t="s">
-        <v>303</v>
-      </c>
-      <c r="B11" s="96" t="s">
+      <c r="C11" s="95" t="s">
         <v>312</v>
       </c>
-      <c r="C11" s="96" t="s">
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="94" t="s">
+        <v>302</v>
+      </c>
+      <c r="B12" s="95" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="95" t="s">
-        <v>303</v>
-      </c>
-      <c r="B12" s="96" t="s">
+      <c r="C12" s="95" t="s">
         <v>314</v>
       </c>
-      <c r="C12" s="96" t="s">
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="94" t="s">
+        <v>302</v>
+      </c>
+      <c r="B13" s="95" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="95" t="s">
-        <v>303</v>
-      </c>
-      <c r="B13" s="96" t="s">
+      <c r="C13" s="95" t="s">
         <v>316</v>
       </c>
-      <c r="C13" s="96" t="s">
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="96" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="97" t="s">
+      <c r="B14" s="44" t="s">
         <v>318</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="C14" s="44" t="s">
         <v>319</v>
       </c>
-      <c r="C14" s="44" t="s">
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="96" t="s">
+        <v>317</v>
+      </c>
+      <c r="B15" s="44" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="97" t="s">
-        <v>318</v>
-      </c>
-      <c r="B15" s="44" t="s">
+      <c r="C15" s="44" t="s">
         <v>321</v>
       </c>
-      <c r="C15" s="44" t="s">
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="96" t="s">
+        <v>317</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>307</v>
+      </c>
+      <c r="C16" s="44" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="97" t="s">
-        <v>318</v>
-      </c>
-      <c r="B16" s="44" t="s">
-        <v>308</v>
-      </c>
-      <c r="C16" s="44" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="96" t="s">
+        <v>317</v>
+      </c>
+      <c r="B17" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="C17" s="44" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="97" t="s">
-        <v>318</v>
-      </c>
-      <c r="B17" s="44" t="s">
-        <v>310</v>
-      </c>
-      <c r="C17" s="44" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" s="96" t="s">
+        <v>317</v>
+      </c>
+      <c r="B18" s="95" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="97" t="s">
-        <v>318</v>
-      </c>
-      <c r="B18" s="96" t="s">
+      <c r="C18" s="95" t="s">
         <v>325</v>
       </c>
-      <c r="C18" s="96" t="s">
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="96" t="s">
+        <v>317</v>
+      </c>
+      <c r="B19" s="95" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="97" t="s">
-        <v>318</v>
-      </c>
-      <c r="B19" s="96" t="s">
+      <c r="C19" s="95" t="s">
         <v>327</v>
       </c>
-      <c r="C19" s="96" t="s">
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="96" t="s">
+        <v>317</v>
+      </c>
+      <c r="B20" s="95" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="97" t="s">
-        <v>318</v>
-      </c>
-      <c r="B20" s="96" t="s">
+      <c r="C20" s="95" t="s">
         <v>329</v>
       </c>
-      <c r="C20" s="96" t="s">
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="96" t="s">
+        <v>317</v>
+      </c>
+      <c r="B21" s="95" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="97" t="s">
-        <v>318</v>
-      </c>
-      <c r="B21" s="96" t="s">
+      <c r="C21" s="95" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="97" t="s">
         <v>331</v>
       </c>
-      <c r="C21" s="96" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="98" t="s">
+      <c r="B22" s="44" t="s">
         <v>332</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="C22" s="45" t="s">
         <v>333</v>
       </c>
-      <c r="C22" s="45" t="s">
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="97" t="s">
+        <v>331</v>
+      </c>
+      <c r="B23" s="44" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="98" t="s">
-        <v>332</v>
-      </c>
-      <c r="B23" s="44" t="s">
+      <c r="C23" s="44" t="s">
         <v>335</v>
       </c>
-      <c r="C23" s="44" t="s">
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="97" t="s">
+        <v>331</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>307</v>
+      </c>
+      <c r="C24" s="44" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="98" t="s">
-        <v>332</v>
-      </c>
-      <c r="B24" s="44" t="s">
-        <v>308</v>
-      </c>
-      <c r="C24" s="44" t="s">
+    <row r="25" spans="1:3">
+      <c r="A25" s="97" t="s">
+        <v>331</v>
+      </c>
+      <c r="B25" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="C25" s="44" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="98" t="s">
-        <v>332</v>
-      </c>
-      <c r="B25" s="44" t="s">
-        <v>310</v>
-      </c>
-      <c r="C25" s="44" t="s">
+    <row r="26" spans="1:3">
+      <c r="A26" s="97" t="s">
+        <v>331</v>
+      </c>
+      <c r="B26" s="44" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="98" t="s">
-        <v>332</v>
-      </c>
-      <c r="B26" s="44" t="s">
+      <c r="C26" s="44" t="s">
         <v>339</v>
       </c>
-      <c r="C26" s="44" t="s">
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="97" t="s">
+        <v>331</v>
+      </c>
+      <c r="B27" s="95" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="98" t="s">
-        <v>332</v>
-      </c>
-      <c r="B27" s="96" t="s">
+      <c r="C27" s="95" t="s">
         <v>341</v>
       </c>
-      <c r="C27" s="96" t="s">
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="97" t="s">
+        <v>331</v>
+      </c>
+      <c r="B28" s="95" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="98" t="s">
-        <v>332</v>
-      </c>
-      <c r="B28" s="96" t="s">
+      <c r="C28" s="95" t="s">
         <v>343</v>
       </c>
-      <c r="C28" s="96" t="s">
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="97" t="s">
+        <v>331</v>
+      </c>
+      <c r="B29" s="95" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="98" t="s">
-        <v>332</v>
-      </c>
-      <c r="B29" s="96" t="s">
+      <c r="C29" s="95" t="s">
         <v>345</v>
       </c>
-      <c r="C29" s="96" t="s">
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="97" t="s">
+        <v>331</v>
+      </c>
+      <c r="B30" s="95" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="98" t="s">
-        <v>332</v>
-      </c>
-      <c r="B30" s="96" t="s">
+      <c r="C30" s="95" t="s">
         <v>347</v>
       </c>
-      <c r="C30" s="96" t="s">
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="98" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="99" t="s">
+      <c r="B31" s="49" t="s">
         <v>349</v>
       </c>
-      <c r="B31" s="49" t="s">
+      <c r="C31" s="49" t="s">
         <v>350</v>
       </c>
-      <c r="C31" s="49" t="s">
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="98" t="s">
+        <v>348</v>
+      </c>
+      <c r="B32" s="49" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="99" t="s">
-        <v>349</v>
-      </c>
-      <c r="B32" s="49" t="s">
+      <c r="C32" s="49" t="s">
         <v>352</v>
       </c>
-      <c r="C32" s="49" t="s">
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="98" t="s">
+        <v>348</v>
+      </c>
+      <c r="B33" s="49" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="99" t="s">
-        <v>349</v>
-      </c>
-      <c r="B33" s="49" t="s">
+      <c r="C33" s="49" t="s">
         <v>354</v>
       </c>
-      <c r="C33" s="49" t="s">
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="98" t="s">
+        <v>348</v>
+      </c>
+      <c r="B34" s="49" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="99" t="s">
-        <v>349</v>
-      </c>
-      <c r="B34" s="49" t="s">
+      <c r="C34" s="49" t="s">
         <v>356</v>
-      </c>
-      <c r="C34" s="49" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B35" s="44" t="s">
-        <v>358</v>
-      </c>
-      <c r="C35" s="102" t="s">
-        <v>372</v>
+        <v>357</v>
+      </c>
+      <c r="C35" s="101" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B36" s="44" t="s">
-        <v>359</v>
-      </c>
-      <c r="C36" s="102" t="s">
-        <v>379</v>
+        <v>358</v>
+      </c>
+      <c r="C36" s="101" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B37" s="44" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C37" s="59" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B38" s="44" t="s">
-        <v>361</v>
-      </c>
-      <c r="C38" s="102" t="s">
-        <v>380</v>
+        <v>360</v>
+      </c>
+      <c r="C38" s="101" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B39" s="44" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C39" s="59" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B40" s="44" t="s">
-        <v>363</v>
-      </c>
-      <c r="C40" s="102" t="s">
-        <v>381</v>
+        <v>362</v>
+      </c>
+      <c r="C40" s="101" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B41" s="44" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C41" s="59" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B42" s="44" t="s">
-        <v>365</v>
-      </c>
-      <c r="C42" s="102" t="s">
-        <v>382</v>
+        <v>364</v>
+      </c>
+      <c r="C42" s="101" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B43" s="44" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C43" s="59" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B44" s="44" t="s">
-        <v>367</v>
-      </c>
-      <c r="C44" s="102" t="s">
-        <v>383</v>
+        <v>366</v>
+      </c>
+      <c r="C44" s="101" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B45" s="44" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C45" s="59" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B46" s="44" t="s">
-        <v>369</v>
-      </c>
-      <c r="C46" s="102" t="s">
-        <v>384</v>
+        <v>368</v>
+      </c>
+      <c r="C46" s="101" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B47" s="44" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C47" s="59" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B48" s="44" t="s">
-        <v>371</v>
-      </c>
-      <c r="C48" s="102" t="s">
-        <v>385</v>
+        <v>370</v>
+      </c>
+      <c r="C48" s="101" t="s">
+        <v>384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>